<commit_message>
Processed another batch of links
And got myself an increased editing limit: 14 sequences at once!
</commit_message>
<xml_diff>
--- a/broken.xlsx
+++ b/broken.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01028734c1c2e442/Рабочий стол/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:40009_{750DEEBC-8306-47E1-A9AD-D352C13D1A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9225A6BE-5C01-45D6-973E-001399B550E1}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="13_ncr:40009_{750DEEBC-8306-47E1-A9AD-D352C13D1A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{601FEC47-6FD4-451E-8F68-0E69BA45EA15}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="1118">
   <si>
     <t>http://14142.net/n-puzzle/document/document.html</t>
   </si>
@@ -2902,9 +2902,6 @@
     <t>http://pollack.uga.edu/multpart.pdf</t>
   </si>
   <si>
-    <t>https://www.ams.org/journals/btran/2016-03-01/S2330-0000-2016-00010-2/S2330-0000-2016-00010-2.pdf</t>
-  </si>
-  <si>
     <t>http://pollack.uga.edu/variations.pdf</t>
   </si>
   <si>
@@ -3058,13 +3055,325 @@
     <t>https://pdfs.semanticscholar.org/301f/777cd44aaa90b1a24c2ddc1d07721bbc9051.pdf</t>
   </si>
   <si>
-    <t>http://www.wisdom.weizmann.ac.il/~fraenkel/Papers/YJCTA4036.pdf</t>
-  </si>
-  <si>
-    <t>https://www.semanticscholar.org/paper/Extensions-and-restrictions-of-Wythoff's-game-its-p-Duch%C3%AAne-Fraenkel/b1e9ee254c6f8ef6b2e07991a0c7286fe5a46dc7</t>
-  </si>
-  <si>
     <t>https://www.researchgate.net/publication/299482951_Digit_And_Iterative_Digit_Sum_Of_Fibonacci_Numbers_Their_Identities_And_Powers</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1902.00815</t>
+  </si>
+  <si>
+    <t>https://opinvisindi.is/bitstream/handle/20.500.11815/1184/phd-bean-2018.pdf?sequence=1</t>
+  </si>
+  <si>
+    <t>http://www.iam.fmph.uniba.sk/amuc/ojs/index.php/amuc/article/view/1307</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1810.06853</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1810.07895</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1810.10391</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1810.10423</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1810.12701</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1810.12975</t>
+  </si>
+  <si>
+    <t>behind paywall</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s11139-017-9988-0</t>
+  </si>
+  <si>
+    <t>https://www.worldscientific.com/doi/abs/10.1142/S1793042120500475</t>
+  </si>
+  <si>
+    <t>http://www.gimnazija-izdijankoveckoga-kc.skole.hr/upload/gimnazija-izdijankoveckoga-kc/multistatic/651/LaurendiPartitions.pdf</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/On-the-parity-of-the-number-of-multiplicative-Zaharescu-Zaki/2f73099c652a7b1ed615772d6434249ddece3962</t>
+  </si>
+  <si>
+    <t>http://jnsilva.ludicum.org/TJ/TJ1920/FamousNumbers.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/math/0505167</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>https://carma.newcastle.edu.au/meetings/alfcon/pdfs/Frank_Garvan-alfcon.pdf</t>
+  </si>
+  <si>
+    <t>https://carma.newcastle.edu.au/resources/jon/wmi-paper.pdf</t>
+  </si>
+  <si>
+    <t>http://users.telenet.be/Wouter.Meeussen/SetPartitionsUpToRotations.nb</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/0911.2683</t>
+  </si>
+  <si>
+    <t>http://www-groups.mcs.st-andrews.ac.uk/~vince/publications/popstacks/pop-stacks.pdf</t>
+  </si>
+  <si>
+    <t>probably redundant</t>
+  </si>
+  <si>
+    <t>https://maths-people.anu.edu.au/~eastwood/fayetteville5.pdf</t>
+  </si>
+  <si>
+    <t>http://carma.newcastle.edu.au/meetings/alfcon/pdfs/Hugh_Williams-alfcon.pdf</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20160323050648/https://www.theophys.kth.se/~phl/Mathematica/</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20150318204102/http://2000clicks.com/mathhelp/PuzzlePowersOf3AndPowersOf2Answer.aspx</t>
+  </si>
+  <si>
+    <t>nowhere to be found</t>
+  </si>
+  <si>
+    <t>L. Hajdu, On a conjecture of Pomerance and the Jacobsthal function, 27th Journées Arithmétiques</t>
+  </si>
+  <si>
+    <t>http://bookre.org/reader?file=550537&amp;pg=43</t>
+  </si>
+  <si>
+    <t>https://math.boisestate.edu/reu/publications/quantifying-cds-sortability.pdf</t>
+  </si>
+  <si>
+    <t>https://pdfslide.net/documents/evil-twins-alternate-with-odious-twins-fairfield-twinspdf-evil-twins-alternate.html</t>
+  </si>
+  <si>
+    <t>N. Magot and A. Zvonkin, Belyi functions for Archimedian solids, Discrete Math., 217 (2000), 249-271.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0012-365X(99)00266-6</t>
+  </si>
+  <si>
+    <t>https://homepages.warwick.ac.uk/staff/J.E.Cremona/book/fulltext/index.html</t>
+  </si>
+  <si>
+    <t>http://friedo.szm.com/krypto/JS/home.ecn.ab.ca/~jsavard/crypto.htm</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Iaroslav_Blagouchine/publication/260672713_Analytic_Method_for_the_Computation_of_the_Total_Harmonic_Distortion_by_the_Cauchy_Method_of_Residues/links/0deec53ca87360a1da000000.pdf</t>
+  </si>
+  <si>
+    <t>http://math.univ-lyon1.fr/homes-www/zeng/public_html/paper/publication.html</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1709.08416</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1610.02965</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Lista_dei_politopi_regolari</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.disc.2014.12.003</t>
+  </si>
+  <si>
+    <t>https://cdn.cs50.net/2010/fall/psets/3/saml.pdf</t>
+  </si>
+  <si>
+    <t>http://list.seqfan.eu/pipermail/seqfan/2015-January/</t>
+  </si>
+  <si>
+    <t>https://www.math.arizona.edu/~ura-reports/053/Moore.Matthew/Final.pdf</t>
+  </si>
+  <si>
+    <t>http://www.math.arizona.edu/~ura-reports/001/gaberdiel.jw/</t>
+  </si>
+  <si>
+    <t>Zhi-Wei Sun, On Divisibility Of Binomial Coefficients, Journal of the Australian Mathematical Society 93 (2012), p. 189-201.</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/arxiv-1005.1054/mode/2up</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1011.6676</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jnt.2013.02.014</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1308.2900</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1102.5649</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1208.2683</t>
+  </si>
+  <si>
+    <t>C. Lanius, The Koch Snowflake</t>
+  </si>
+  <si>
+    <t>M. Eastwood, The X-ray transform on projective space</t>
+  </si>
+  <si>
+    <t>https://www.math.uci.edu/~krubin/lectures/rossweb.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ralph E. Griswold, Shaft Sequences </t>
+  </si>
+  <si>
+    <t>https://www2.cs.arizona.edu/patterns/sequences/</t>
+  </si>
+  <si>
+    <t>K. Sutner, The Ehrenfeucht-Mycielski sequence</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/3-540-45089-0_26</t>
+  </si>
+  <si>
+    <t>https://inference.org.uk/mackay/abstracts/sumsquares.html</t>
+  </si>
+  <si>
+    <t>Saleem Bhatti, Channel coding; Hamming distance</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/235711311_Degrees_of_Streams</t>
+  </si>
+  <si>
+    <t>V. L. Almstrum, Visual Koch (Applet)</t>
+  </si>
+  <si>
+    <t>D. J. C. Mackay and S. Mahajan, Numbers that are Sums of Squares in Several Ways</t>
+  </si>
+  <si>
+    <t>http://docplayer.net/87034980-Vol-15-no-2-april-2017-dmmmsu-cas-science-monitor.html</t>
+  </si>
+  <si>
+    <t>https://tromp.github.io/go.html</t>
+  </si>
+  <si>
+    <t>Dik T. Winter, Armstrong numbers</t>
+  </si>
+  <si>
+    <t>Andrew Reiter, On (mod n) spirals</t>
+  </si>
+  <si>
+    <t>R. Sprugnoli, Riordan Array Proofs of Identities in Gould's Book.</t>
+  </si>
+  <si>
+    <t>R. Sprugnoli, Riordan array proofs of identities in Gould's book</t>
+  </si>
+  <si>
+    <t>T. A. Gulliver, Sequences from Arrays of Integers</t>
+  </si>
+  <si>
+    <t>Walter Arrighetti, Double Vision</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/math/0310132</t>
+  </si>
+  <si>
+    <t>K. S. Immink, Coding Schemes for Multi-Level Channels that are Intrinsically Resistant Against Unknown Gain and/or Offset Using Reference Symbols</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20191223050847/https://garlic.com/~wedgingt/mersenne.html</t>
+  </si>
+  <si>
+    <t>https://people.mpim-bonn.mpg.de/moree/Moree-details.en.shtml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E. V. Yatziv, Overview of Hebrew Language Structure </t>
+  </si>
+  <si>
+    <t>http://www.arves.org/arves/images/PDF/EG_PDF/eg73.pdf</t>
+  </si>
+  <si>
+    <t>http://fumba.eu/sitelayout/Floretion.php</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20030211053857/https://frii.com/~dboll/packing.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://doi.org/10.1007/978-3-0348-8405-1_11</t>
+  </si>
+  <si>
+    <t>should be deleted, not fixed</t>
+  </si>
+  <si>
+    <t>fixed, thanks to Erich</t>
+  </si>
+  <si>
+    <t>https://utm.edu/staff/caldwell/preprints/6521.pdf</t>
+  </si>
+  <si>
+    <t>https://www-fourier.univ-grenoble-alpes.fr/?q=fr/content/reseaux-entiers-unimodulaires-sans-racine-en-dimension-27-et-28</t>
+  </si>
+  <si>
+    <t>wrote to dr. Herzog, waiting for an answer</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/BF02854385</t>
+  </si>
+  <si>
+    <t>https://orbi.uliege.be/bitstream/2268/100440/2/Wythoff-adj2.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1090/btran/10</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/On-extremal-cases-of-pop-stack-sorting-Asinowski/4b17b76c31559d6d8126b8f1126fdb357f3a5df0</t>
+  </si>
+  <si>
+    <t>http://digitalcommons.plattsburgh.edu/mathematics_facpubs/9/</t>
+  </si>
+  <si>
+    <t>http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.530.857</t>
+  </si>
+  <si>
+    <t>https://skepticalinquirer.org/1998/09/coincidences-remarkable-or-random/</t>
+  </si>
+  <si>
+    <t>https://pdfslide.net/documents/the-square-pyramidal-number-and-other-figurate-numbers.html</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/Restricted-Symmetric-Signed-Permutations-Hardt/d9c774e4c5850d6478c3153e2794d9f50f5cbad8</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/Meander-Graphs-and-Frobenius-Seaweed-Lie-Algebras-Coll-Hyatt/617f240bbafa65eed819c991c7a6cb93544ceba2</t>
+  </si>
+  <si>
+    <t>S. S. Pillai, On a congruence property of the divisor function, J. Indian Math. Soc. (N. S.), Vol. 6, (1942), pp. 118-119.</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/Performances-of-Multi-Level-and-Multi-Component-Wu-Stockinger/86df33afe20a167445d73111af9d49cb63d17fe2</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20190529184441/https://centerforbookarts.org/tuesday-typefaces-times-new-roman/</t>
+  </si>
+  <si>
+    <t>http://users.rowan.edu/%7Esimons/abundant.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.14708/wm.v47i2.192</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/An-Average-Case-Analysis-of-the-Gaussian-Algorithm-Daud%C3%A9-Flajolet/5783d4bfc398819b106c216bfea14347dd58550b</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2006.14070</t>
+  </si>
+  <si>
+    <t>http://www.gabrielnivasch.org/fun/combinatorial-games/sprague-grundy</t>
+  </si>
+  <si>
+    <t>https://www.ejournals.eu/sj/index.php/SI/article/view/2227</t>
   </si>
 </sst>
 </file>
@@ -3581,12 +3890,16 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -3650,7 +3963,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F1000" totalsRowShown="0">
   <autoFilter ref="A1:F1000" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F789">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F787">
     <sortCondition ref="A1:A1000"/>
   </sortState>
   <tableColumns count="6">
@@ -3962,10 +4275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F787"/>
+  <dimension ref="A1:F788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A774" workbookViewId="0">
-      <selection activeCell="A784" sqref="A784"/>
+    <sheetView tabSelected="1" topLeftCell="A667" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A678" sqref="A678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4007,11 +4320,20 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="E4" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -4023,10 +4345,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C6" t="s">
-        <v>964</v>
+        <v>963</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4050,16 +4375,19 @@
       <c r="C8" t="s">
         <v>959</v>
       </c>
+      <c r="F8" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D9" t="s">
-        <v>960</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4067,10 +4395,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C10" t="s">
-        <v>961</v>
+        <v>960</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4083,6 +4414,9 @@
       <c r="C11" t="s">
         <v>867</v>
       </c>
+      <c r="F11" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -4094,6 +4428,9 @@
       <c r="C12" t="s">
         <v>868</v>
       </c>
+      <c r="F12" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -4105,11 +4442,20 @@
       <c r="C13" t="s">
         <v>870</v>
       </c>
+      <c r="F13" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1039</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -4121,90 +4467,105 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="C24" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="C25" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="C32" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="F32" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -4212,52 +4573,58 @@
         <v>873</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="C39" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -4265,12 +4632,12 @@
         <v>874</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4280,8 +4647,11 @@
       <c r="C45" s="1" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="F45" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -4289,7 +4659,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -4297,7 +4667,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -4422,6 +4792,9 @@
       <c r="A62" t="s">
         <v>60</v>
       </c>
+      <c r="D62" t="s">
+        <v>1043</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
@@ -4433,92 +4806,101 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -4526,12 +4908,12 @@
         <v>837</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -4541,8 +4923,11 @@
       <c r="D84" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="F84" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -4553,7 +4938,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -4564,218 +4949,288 @@
         <v>844</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="4" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="F87" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="D88" s="4"/>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="D89" s="4"/>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="D90" s="4"/>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="C91" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D91" s="4"/>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="C95" s="5" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="D98" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="C99" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="D100" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="D101" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="C106" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
+      <c r="D107" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="D110" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="C113" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="C117" s="1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="C118" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D121" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="D122" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="D123" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="D124" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="D125" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="D126" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -4819,11 +5274,20 @@
       <c r="A133" t="s">
         <v>115</v>
       </c>
+      <c r="D133" t="s">
+        <v>1067</v>
+      </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>132</v>
       </c>
+      <c r="B134" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1035</v>
+      </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
@@ -4884,7 +5348,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -4892,7 +5356,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:6">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -4900,7 +5364,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -4908,7 +5372,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>145</v>
       </c>
@@ -4916,15 +5380,18 @@
         <v>800</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>146</v>
       </c>
       <c r="C149" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="F149" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>147</v>
       </c>
@@ -4932,7 +5399,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>148</v>
       </c>
@@ -4940,7 +5407,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:6">
       <c r="A152" s="1" t="s">
         <v>149</v>
       </c>
@@ -4948,7 +5415,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>155</v>
       </c>
@@ -4956,7 +5423,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:6">
       <c r="A154" s="1" t="s">
         <v>150</v>
       </c>
@@ -4964,7 +5431,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>151</v>
       </c>
@@ -4972,7 +5439,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -4980,7 +5447,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>153</v>
       </c>
@@ -4988,17 +5455,17 @@
         <v>793</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -5312,7 +5779,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:6">
       <c r="A209" t="s">
         <v>207</v>
       </c>
@@ -5320,7 +5787,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:6">
       <c r="A210" t="s">
         <v>208</v>
       </c>
@@ -5328,7 +5795,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:6">
       <c r="A211" t="s">
         <v>209</v>
       </c>
@@ -5336,7 +5803,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:6">
       <c r="A212" t="s">
         <v>210</v>
       </c>
@@ -5344,7 +5811,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:6">
       <c r="A213" t="s">
         <v>211</v>
       </c>
@@ -5352,7 +5819,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:6">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -5360,7 +5827,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:6">
       <c r="A215" t="s">
         <v>212</v>
       </c>
@@ -5368,7 +5835,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:6">
       <c r="A216" t="s">
         <v>214</v>
       </c>
@@ -5376,7 +5843,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:6">
       <c r="A217" t="s">
         <v>215</v>
       </c>
@@ -5384,20 +5851,23 @@
         <v>883</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:6">
       <c r="A218" t="s">
         <v>216</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="219" spans="1:3">
+      <c r="F218" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
       <c r="A219" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:6">
       <c r="A220" t="s">
         <v>218</v>
       </c>
@@ -5407,23 +5877,26 @@
       <c r="C220" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="221" spans="1:3">
+      <c r="F220" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
       <c r="A221" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:6">
       <c r="A222" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:6">
       <c r="A223" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:6">
       <c r="A224" t="s">
         <v>222</v>
       </c>
@@ -5501,11 +5974,17 @@
       <c r="A237" t="s">
         <v>235</v>
       </c>
+      <c r="D237" t="s">
+        <v>1032</v>
+      </c>
     </row>
     <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>236</v>
       </c>
+      <c r="D238" t="s">
+        <v>1033</v>
+      </c>
     </row>
     <row r="239" spans="1:5">
       <c r="A239" t="s">
@@ -5517,76 +5996,85 @@
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:6">
       <c r="A241" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="242" spans="1:5">
+      <c r="C241" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
       <c r="A242" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:6">
       <c r="A243" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="244" spans="1:5">
+      <c r="F243" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
       <c r="A244" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:6">
       <c r="A245" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:6">
       <c r="A246" t="s">
         <v>244</v>
       </c>
       <c r="E246" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6">
       <c r="A247" t="s">
         <v>246</v>
       </c>
       <c r="C247" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5">
+        <v>965</v>
+      </c>
+      <c r="F247" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6">
       <c r="A248" t="s">
         <v>245</v>
       </c>
       <c r="C248" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6">
       <c r="A249" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:6">
       <c r="A250" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:6">
       <c r="A251" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:6">
       <c r="A252" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:6">
       <c r="A253" t="s">
         <v>251</v>
       </c>
@@ -5594,97 +6082,100 @@
         <v>905</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:6">
       <c r="A254" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="255" spans="1:5">
+    <row r="255" spans="1:6">
       <c r="A255" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:6">
       <c r="A256" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="257" spans="1:1">
+    <row r="257" spans="1:4">
       <c r="A257" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="258" spans="1:1">
+    <row r="258" spans="1:4">
       <c r="A258" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="259" spans="1:1">
+    <row r="259" spans="1:4">
       <c r="A259" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="260" spans="1:1">
+    <row r="260" spans="1:4">
       <c r="A260" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="261" spans="1:1">
+    <row r="261" spans="1:4">
       <c r="A261" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="262" spans="1:1">
+    <row r="262" spans="1:4">
       <c r="A262" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="263" spans="1:1">
+    <row r="263" spans="1:4">
       <c r="A263" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="264" spans="1:1">
+    <row r="264" spans="1:4">
       <c r="A264" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="265" spans="1:1">
+      <c r="D264" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
       <c r="A265" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="266" spans="1:1">
+    <row r="266" spans="1:4">
       <c r="A266" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="267" spans="1:1">
+    <row r="267" spans="1:4">
       <c r="A267" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="268" spans="1:1">
+    <row r="268" spans="1:4">
       <c r="A268" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="269" spans="1:1">
+    <row r="269" spans="1:4">
       <c r="A269" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="270" spans="1:1">
+    <row r="270" spans="1:4">
       <c r="A270" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="271" spans="1:1">
+    <row r="271" spans="1:4">
       <c r="A271" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="272" spans="1:1">
+    <row r="272" spans="1:4">
       <c r="A272" t="s">
         <v>275</v>
       </c>
@@ -5894,107 +6385,146 @@
         <v>307</v>
       </c>
     </row>
-    <row r="305" spans="1:1">
+    <row r="305" spans="1:4">
       <c r="A305" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="306" spans="1:1">
+      <c r="B305" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
       <c r="A306" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="307" spans="1:1">
+      <c r="B306" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
       <c r="A307" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="308" spans="1:1">
+    <row r="308" spans="1:4">
       <c r="A308" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="309" spans="1:1">
+    <row r="309" spans="1:4">
       <c r="A309" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="310" spans="1:1">
+    <row r="310" spans="1:4">
       <c r="A310" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="311" spans="1:1">
+      <c r="B310" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D310" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
       <c r="A311" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="312" spans="1:1">
+      <c r="B311" s="1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
       <c r="A312" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="313" spans="1:1">
+      <c r="B312" s="3" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4">
       <c r="A313" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="314" spans="1:1">
+    <row r="314" spans="1:4">
       <c r="A314" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="315" spans="1:1">
-      <c r="A315" t="s">
+    <row r="315" spans="1:4">
+      <c r="A315" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="316" spans="1:1">
+      <c r="D315" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
       <c r="A316" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:4">
       <c r="A317" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:4">
       <c r="A318" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="319" spans="1:1">
+      <c r="B318" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4">
       <c r="A319" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="320" spans="1:1">
+      <c r="B319" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4">
       <c r="A320" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="321" spans="1:3">
+      <c r="C320" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6">
       <c r="A321" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:6">
       <c r="A322" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:6">
       <c r="A323" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="324" spans="1:3">
+      <c r="D323" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6">
       <c r="A324" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:6">
       <c r="A325" t="s">
         <v>328</v>
       </c>
@@ -6004,8 +6534,11 @@
       <c r="C325" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="326" spans="1:3">
+      <c r="F325" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6">
       <c r="A326" t="s">
         <v>329</v>
       </c>
@@ -6015,8 +6548,11 @@
       <c r="C326" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="327" spans="1:3">
+      <c r="F326" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6">
       <c r="A327" t="s">
         <v>330</v>
       </c>
@@ -6027,7 +6563,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:6">
       <c r="A328" t="s">
         <v>331</v>
       </c>
@@ -6038,7 +6574,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:6">
       <c r="A329" t="s">
         <v>332</v>
       </c>
@@ -6049,7 +6585,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:6">
       <c r="A330" t="s">
         <v>333</v>
       </c>
@@ -6060,7 +6596,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:6">
       <c r="A331" t="s">
         <v>334</v>
       </c>
@@ -6071,7 +6607,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:6">
       <c r="A332" t="s">
         <v>335</v>
       </c>
@@ -6082,197 +6618,266 @@
         <v>932</v>
       </c>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:6">
       <c r="A333" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:6">
       <c r="A334" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:6">
       <c r="A335" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:6">
       <c r="A336" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="337" spans="1:1">
+      <c r="B336" s="1" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6">
       <c r="A337" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="338" spans="1:1">
+      <c r="D337" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F337" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6">
       <c r="A338" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="339" spans="1:1">
+      <c r="B338" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6">
       <c r="A339" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="340" spans="1:1">
+      <c r="B339" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6">
       <c r="A340" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="341" spans="1:1">
+    <row r="341" spans="1:6">
       <c r="A341" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="342" spans="1:1">
+    <row r="342" spans="1:6">
       <c r="A342" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="343" spans="1:1">
+    <row r="343" spans="1:6">
       <c r="A343" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="344" spans="1:1">
+      <c r="B343" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6">
       <c r="A344" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="345" spans="1:1">
+      <c r="F344" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6">
       <c r="A345" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="346" spans="1:1">
+      <c r="F345" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6">
       <c r="A346" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="347" spans="1:1">
+      <c r="F346" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6">
       <c r="A347" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="348" spans="1:1">
+      <c r="B347" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6">
       <c r="A348" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="349" spans="1:1">
+    <row r="349" spans="1:6">
       <c r="A349" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="350" spans="1:1">
+    <row r="350" spans="1:6">
       <c r="A350" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="351" spans="1:1">
+    <row r="351" spans="1:6">
       <c r="A351" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="352" spans="1:1">
+      <c r="D351" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6">
       <c r="A352" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="353" spans="1:3">
+      <c r="E352" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6">
       <c r="A353" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="354" spans="1:3">
+      <c r="C353" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6">
       <c r="A354" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="355" spans="1:3">
+    <row r="355" spans="1:6">
       <c r="A355" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="356" spans="1:3">
+      <c r="C355" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F355" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6">
       <c r="A356" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="357" spans="1:3">
+      <c r="E356" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6">
       <c r="A357" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="358" spans="1:3">
+      <c r="E357" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6">
       <c r="A358" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="359" spans="1:3">
+    <row r="359" spans="1:6">
       <c r="A359" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="360" spans="1:3">
+      <c r="B359" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6">
       <c r="A360" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="361" spans="1:3">
+      <c r="D360" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6">
       <c r="A361" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="362" spans="1:3">
+      <c r="D361" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F361" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6">
       <c r="A362" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="363" spans="1:3">
+    <row r="363" spans="1:6">
       <c r="A363" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="364" spans="1:3">
+    <row r="364" spans="1:6">
       <c r="A364" t="s">
         <v>369</v>
       </c>
       <c r="C364" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="365" spans="1:3">
+        <v>968</v>
+      </c>
+      <c r="F364" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6">
       <c r="A365" t="s">
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="366" spans="1:3">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6">
       <c r="A366" t="s">
         <v>370</v>
       </c>
       <c r="C366" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="367" spans="1:3">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6">
       <c r="A367" t="s">
         <v>368</v>
       </c>
       <c r="B367" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="C367" t="s">
         <v>971</v>
       </c>
-      <c r="C367" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="368" spans="1:3">
+      <c r="F367" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6">
       <c r="A368" t="s">
         <v>371</v>
       </c>
@@ -6911,10 +7516,10 @@
         <v>482</v>
       </c>
       <c r="B478" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="E478" t="s">
         <v>973</v>
-      </c>
-      <c r="E478" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="479" spans="1:5">
@@ -6922,7 +7527,7 @@
         <v>483</v>
       </c>
       <c r="E479" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="480" spans="1:5">
@@ -6930,7 +7535,7 @@
         <v>487</v>
       </c>
       <c r="E480" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="481" spans="1:5">
@@ -6938,7 +7543,7 @@
         <v>484</v>
       </c>
       <c r="E481" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="482" spans="1:5">
@@ -6946,7 +7551,7 @@
         <v>485</v>
       </c>
       <c r="E482" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="483" spans="1:5">
@@ -6954,7 +7559,7 @@
         <v>486</v>
       </c>
       <c r="E483" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="484" spans="1:5">
@@ -6982,7 +7587,7 @@
         <v>492</v>
       </c>
       <c r="D488" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="489" spans="1:5">
@@ -6990,7 +7595,7 @@
         <v>493</v>
       </c>
       <c r="C489" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="490" spans="1:5">
@@ -6998,7 +7603,7 @@
         <v>494</v>
       </c>
       <c r="C490" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="491" spans="1:5">
@@ -7006,7 +7611,7 @@
         <v>495</v>
       </c>
       <c r="C491" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="492" spans="1:5">
@@ -7014,7 +7619,7 @@
         <v>496</v>
       </c>
       <c r="C492" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -7022,7 +7627,7 @@
         <v>497</v>
       </c>
       <c r="C493" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="494" spans="1:5">
@@ -7115,7 +7720,7 @@
         <v>514</v>
       </c>
       <c r="C511" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -7123,7 +7728,7 @@
         <v>515</v>
       </c>
       <c r="C512" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -7131,7 +7736,7 @@
         <v>516</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -7139,7 +7744,7 @@
         <v>517</v>
       </c>
       <c r="C514" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="515" spans="1:3">
@@ -7147,7 +7752,7 @@
         <v>518</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="516" spans="1:3">
@@ -7461,117 +8066,120 @@
         <v>579</v>
       </c>
     </row>
-    <row r="577" spans="1:1">
+    <row r="577" spans="1:4">
       <c r="A577" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="578" spans="1:1">
+    <row r="578" spans="1:4">
       <c r="A578" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="579" spans="1:1">
+    <row r="579" spans="1:4">
       <c r="A579" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="580" spans="1:1">
+    <row r="580" spans="1:4">
       <c r="A580" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="581" spans="1:1">
+    <row r="581" spans="1:4">
       <c r="A581" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="582" spans="1:1">
+    <row r="582" spans="1:4">
       <c r="A582" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="583" spans="1:1">
+    <row r="583" spans="1:4">
       <c r="A583" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="584" spans="1:1">
+    <row r="584" spans="1:4">
       <c r="A584" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="585" spans="1:1">
+    <row r="585" spans="1:4">
       <c r="A585" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="586" spans="1:1">
+    <row r="586" spans="1:4">
       <c r="A586" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="587" spans="1:1">
+      <c r="D586" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4">
       <c r="A587" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="588" spans="1:1">
+    <row r="588" spans="1:4">
       <c r="A588" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="589" spans="1:1">
+    <row r="589" spans="1:4">
       <c r="A589" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="590" spans="1:1">
+    <row r="590" spans="1:4">
       <c r="A590" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="591" spans="1:1">
+    <row r="591" spans="1:4">
       <c r="A591" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="592" spans="1:1">
+    <row r="592" spans="1:4">
       <c r="A592" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="593" spans="1:5">
+    <row r="593" spans="1:6">
       <c r="A593" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="594" spans="1:5">
+    <row r="594" spans="1:6">
       <c r="A594" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="595" spans="1:5">
+    <row r="595" spans="1:6">
       <c r="A595" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="596" spans="1:5">
+    <row r="596" spans="1:6">
       <c r="A596" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="597" spans="1:5">
+    <row r="597" spans="1:6">
       <c r="A597" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="598" spans="1:5">
+    <row r="598" spans="1:6">
       <c r="A598" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="599" spans="1:5">
+    <row r="599" spans="1:6">
       <c r="A599" t="s">
         <v>602</v>
       </c>
@@ -7579,15 +8187,18 @@
         <v>952</v>
       </c>
     </row>
-    <row r="600" spans="1:5">
+    <row r="600" spans="1:6">
       <c r="A600" t="s">
         <v>603</v>
       </c>
       <c r="C600" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="601" spans="1:5">
+      <c r="F600" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6">
       <c r="A601" t="s">
         <v>604</v>
       </c>
@@ -7595,43 +8206,46 @@
         <v>950</v>
       </c>
     </row>
-    <row r="602" spans="1:5">
+    <row r="602" spans="1:6">
       <c r="A602" t="s">
         <v>605</v>
       </c>
       <c r="C602" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="603" spans="1:5">
+      <c r="F602" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6">
       <c r="A603" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="604" spans="1:5">
+    <row r="604" spans="1:6">
       <c r="A604" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="605" spans="1:5">
+    <row r="605" spans="1:6">
       <c r="A605" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="606" spans="1:5">
+    <row r="606" spans="1:6">
       <c r="A606" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="607" spans="1:5">
+    <row r="607" spans="1:6">
       <c r="A607" t="s">
         <v>610</v>
       </c>
       <c r="E607" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="608" spans="1:5">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6">
       <c r="A608" t="s">
         <v>611</v>
       </c>
@@ -7641,7 +8255,7 @@
         <v>612</v>
       </c>
       <c r="E609" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="610" spans="1:5">
@@ -7649,7 +8263,7 @@
         <v>613</v>
       </c>
       <c r="E610" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="611" spans="1:5">
@@ -7668,8 +8282,11 @@
       </c>
     </row>
     <row r="614" spans="1:5">
-      <c r="A614" t="s">
+      <c r="A614" s="1" t="s">
         <v>617</v>
+      </c>
+      <c r="D614" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="615" spans="1:5">
@@ -7677,7 +8294,7 @@
         <v>618</v>
       </c>
       <c r="D615" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="616" spans="1:5">
@@ -7725,12 +8342,12 @@
         <v>627</v>
       </c>
     </row>
-    <row r="625" spans="1:4">
+    <row r="625" spans="1:6">
       <c r="A625" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="626" spans="1:4">
+    <row r="626" spans="1:6">
       <c r="A626" t="s">
         <v>629</v>
       </c>
@@ -7738,7 +8355,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="627" spans="1:4">
+    <row r="627" spans="1:6">
       <c r="A627" t="s">
         <v>630</v>
       </c>
@@ -7746,80 +8363,113 @@
         <v>955</v>
       </c>
     </row>
-    <row r="628" spans="1:4">
+    <row r="628" spans="1:6">
       <c r="A628" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="629" spans="1:4">
+    <row r="629" spans="1:6">
       <c r="A629" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="630" spans="1:4">
+    <row r="630" spans="1:6">
       <c r="A630" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="631" spans="1:4">
+    <row r="631" spans="1:6">
       <c r="A631" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="632" spans="1:4">
+    <row r="632" spans="1:6">
       <c r="A632" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="633" spans="1:4">
+      <c r="F632" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6">
       <c r="A633" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="634" spans="1:4">
+      <c r="F633" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6">
       <c r="A634" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="635" spans="1:4">
+      <c r="F634" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6">
       <c r="A635" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="636" spans="1:4">
+      <c r="F635" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6">
       <c r="A636" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="637" spans="1:4">
+      <c r="F636" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6">
       <c r="A637" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="638" spans="1:4">
+      <c r="F637" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6">
       <c r="A638" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="639" spans="1:4">
+      <c r="F638" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6">
       <c r="A639" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="640" spans="1:4">
+      <c r="F639" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6">
       <c r="A640" t="s">
         <v>643</v>
+      </c>
+      <c r="F640" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="641" spans="1:6">
       <c r="A641" t="s">
         <v>644</v>
       </c>
+      <c r="F641" t="s">
+        <v>1095</v>
+      </c>
     </row>
     <row r="642" spans="1:6">
       <c r="A642" t="s">
         <v>645</v>
       </c>
+      <c r="F642" t="s">
+        <v>1095</v>
+      </c>
     </row>
     <row r="643" spans="1:6">
       <c r="A643" t="s">
@@ -7856,10 +8506,10 @@
         <v>652</v>
       </c>
       <c r="E649" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F649" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="650" spans="1:6">
@@ -7870,7 +8520,7 @@
         <v>902</v>
       </c>
       <c r="F650" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="651" spans="1:6">
@@ -7878,10 +8528,10 @@
         <v>654</v>
       </c>
       <c r="E651" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F651" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="652" spans="1:6">
@@ -7889,10 +8539,10 @@
         <v>655</v>
       </c>
       <c r="E652" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F652" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="653" spans="1:6">
@@ -7900,10 +8550,10 @@
         <v>656</v>
       </c>
       <c r="E653" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F653" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="654" spans="1:6">
@@ -7911,10 +8561,10 @@
         <v>657</v>
       </c>
       <c r="E654" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="F654" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="655" spans="1:6">
@@ -7922,7 +8572,7 @@
         <v>658</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="656" spans="1:6">
@@ -7930,97 +8580,103 @@
         <v>659</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="657" spans="1:3">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="657" spans="1:6">
       <c r="A657" t="s">
         <v>660</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="658" spans="1:3">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="658" spans="1:6">
       <c r="A658" t="s">
         <v>661</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="659" spans="1:3">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="659" spans="1:6">
       <c r="A659" t="s">
         <v>662</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="660" spans="1:3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="660" spans="1:6">
       <c r="A660" t="s">
         <v>663</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="661" spans="1:3">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="661" spans="1:6">
       <c r="A661" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="662" spans="1:3">
+    <row r="662" spans="1:6">
       <c r="A662" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="663" spans="1:3">
+    <row r="663" spans="1:6">
       <c r="A663" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="664" spans="1:3">
+    <row r="664" spans="1:6">
       <c r="A664" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="665" spans="1:3">
+    <row r="665" spans="1:6">
       <c r="A665" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="666" spans="1:3">
+    <row r="666" spans="1:6">
       <c r="A666" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="667" spans="1:3">
+    <row r="667" spans="1:6">
       <c r="A667" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="668" spans="1:3">
+    <row r="668" spans="1:6">
       <c r="A668" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="669" spans="1:3">
+      <c r="C668" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F668" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="669" spans="1:6">
       <c r="A669" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="670" spans="1:3">
+    <row r="670" spans="1:6">
       <c r="A670" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="671" spans="1:3">
+    <row r="671" spans="1:6">
       <c r="A671" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="672" spans="1:3">
+    <row r="672" spans="1:6">
       <c r="A672" t="s">
         <v>675</v>
       </c>
@@ -8036,7 +8692,7 @@
       </c>
     </row>
     <row r="675" spans="1:1">
-      <c r="A675" t="s">
+      <c r="A675" s="1" t="s">
         <v>678</v>
       </c>
     </row>
@@ -8185,327 +8841,459 @@
         <v>707</v>
       </c>
     </row>
-    <row r="705" spans="1:1">
+    <row r="705" spans="1:6">
       <c r="A705" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="706" spans="1:1">
+    <row r="706" spans="1:6">
       <c r="A706" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="707" spans="1:1">
+    <row r="707" spans="1:6">
       <c r="A707" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="708" spans="1:1">
+    <row r="708" spans="1:6">
       <c r="A708" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="709" spans="1:1">
+    <row r="709" spans="1:6">
       <c r="A709" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="710" spans="1:1">
+    <row r="710" spans="1:6">
       <c r="A710" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="711" spans="1:1">
+    <row r="711" spans="1:6">
       <c r="A711" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="712" spans="1:1">
+    <row r="712" spans="1:6">
       <c r="A712" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="713" spans="1:1">
+    <row r="713" spans="1:6">
       <c r="A713" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="714" spans="1:1">
+    <row r="714" spans="1:6">
       <c r="A714" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="715" spans="1:1">
+    <row r="715" spans="1:6">
       <c r="A715" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="716" spans="1:1">
+      <c r="D715" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="716" spans="1:6">
       <c r="A716" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="717" spans="1:1">
+    <row r="717" spans="1:6">
       <c r="A717" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="718" spans="1:1">
+      <c r="C717" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="718" spans="1:6">
       <c r="A718" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="719" spans="1:1">
+      <c r="D718" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F718" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="719" spans="1:6">
       <c r="A719" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="720" spans="1:1">
+      <c r="F719" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="720" spans="1:6">
       <c r="A720" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="721" spans="1:1">
+      <c r="F720" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="721" spans="1:6">
       <c r="A721" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="722" spans="1:1">
+      <c r="F721" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="722" spans="1:6">
       <c r="A722" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="723" spans="1:1">
+      <c r="F722" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="723" spans="1:6">
       <c r="A723" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="724" spans="1:1">
+      <c r="F723" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="724" spans="1:6">
       <c r="A724" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="725" spans="1:1">
+      <c r="F724" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="725" spans="1:6">
       <c r="A725" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="726" spans="1:1">
+      <c r="F725" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="726" spans="1:6">
       <c r="A726" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="727" spans="1:1">
+      <c r="F726" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="727" spans="1:6">
       <c r="A727" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="728" spans="1:1">
+      <c r="F727" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="728" spans="1:6">
       <c r="A728" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="729" spans="1:1">
+      <c r="F728" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="729" spans="1:6">
       <c r="A729" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="730" spans="1:1">
+    <row r="730" spans="1:6">
       <c r="A730" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="731" spans="1:1">
+      <c r="C730" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F730" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="731" spans="1:6">
       <c r="A731" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="732" spans="1:1">
+      <c r="C731" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F731" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="732" spans="1:6">
       <c r="A732" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="733" spans="1:1">
+      <c r="D732" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="733" spans="1:6">
       <c r="A733" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="734" spans="1:1">
+      <c r="D733" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="734" spans="1:6">
       <c r="A734" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="735" spans="1:1">
+      <c r="D734" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="735" spans="1:6">
       <c r="A735" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="736" spans="1:1">
+      <c r="F735" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="736" spans="1:6">
       <c r="A736" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="737" spans="1:1">
+      <c r="C736" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="737" spans="1:6">
       <c r="A737" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="738" spans="1:1">
+      <c r="C737" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="738" spans="1:6">
       <c r="A738" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="739" spans="1:1">
+      <c r="C738" s="1" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="739" spans="1:6">
       <c r="A739" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="740" spans="1:1">
+      <c r="C739" s="1" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="740" spans="1:6">
       <c r="A740" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="741" spans="1:1">
+      <c r="C740" s="1" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="741" spans="1:6">
       <c r="A741" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="742" spans="1:1">
+      <c r="C741" s="1" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="742" spans="1:6">
       <c r="A742" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="743" spans="1:1">
+      <c r="C742" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F742" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="743" spans="1:6">
       <c r="A743" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="744" spans="1:1">
+      <c r="D743" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F743" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="744" spans="1:6">
       <c r="A744" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="745" spans="1:1">
+      <c r="D744" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="745" spans="1:6">
       <c r="A745" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="746" spans="1:1">
+      <c r="E745" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="746" spans="1:6">
       <c r="A746" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="747" spans="1:1">
+    <row r="747" spans="1:6">
       <c r="A747" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="748" spans="1:1">
+      <c r="D747" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="748" spans="1:6">
       <c r="A748" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="749" spans="1:1">
+    <row r="749" spans="1:6">
       <c r="A749" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="750" spans="1:1">
+    <row r="750" spans="1:6">
       <c r="A750" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="751" spans="1:1">
+    <row r="751" spans="1:6">
       <c r="A751" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="752" spans="1:1">
+    <row r="752" spans="1:6">
       <c r="A752" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="753" spans="1:3">
+      <c r="C752" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F752" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6">
       <c r="A753" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="754" spans="1:3">
+      <c r="C753" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F753" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="754" spans="1:6">
       <c r="A754" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="755" spans="1:3">
+      <c r="C754" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F754" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6">
       <c r="A755" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="756" spans="1:3">
+    <row r="756" spans="1:6">
       <c r="A756" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="757" spans="1:3">
+    <row r="757" spans="1:6">
       <c r="A757" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="758" spans="1:3">
+      <c r="B757" s="1" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6">
       <c r="A758" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="759" spans="1:3">
+      <c r="D758" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6">
       <c r="A759" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="760" spans="1:3">
+    <row r="760" spans="1:6">
       <c r="A760" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="761" spans="1:3">
+    <row r="761" spans="1:6">
       <c r="A761" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="762" spans="1:3">
+    <row r="762" spans="1:6">
       <c r="A762" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="763" spans="1:3">
+    <row r="763" spans="1:6">
       <c r="A763" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="764" spans="1:3">
+    <row r="764" spans="1:6">
       <c r="A764" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="765" spans="1:3">
+    <row r="765" spans="1:6">
       <c r="A765" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="766" spans="1:3">
+      <c r="D765" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="766" spans="1:6">
       <c r="A766" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="767" spans="1:3">
+    <row r="767" spans="1:6">
       <c r="A767" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="768" spans="1:3">
+    <row r="768" spans="1:6">
       <c r="A768" t="s">
         <v>766</v>
       </c>
       <c r="C768" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="769" spans="1:6">
@@ -8513,7 +9301,7 @@
         <v>767</v>
       </c>
       <c r="C769" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="770" spans="1:6">
@@ -8521,10 +9309,10 @@
         <v>768</v>
       </c>
       <c r="C770" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F770" t="s">
         <v>1009</v>
-      </c>
-      <c r="F770" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="771" spans="1:6">
@@ -8532,34 +9320,46 @@
         <v>769</v>
       </c>
       <c r="C771" t="s">
-        <v>1011</v>
+        <v>1010</v>
+      </c>
+      <c r="F771" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="772" spans="1:6">
       <c r="A772" t="s">
         <v>770</v>
       </c>
-      <c r="C772" t="s">
-        <v>1013</v>
-      </c>
       <c r="D772" t="s">
-        <v>1012</v>
+        <v>1100</v>
+      </c>
+      <c r="F772" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="773" spans="1:6">
       <c r="A773" t="s">
         <v>771</v>
       </c>
+      <c r="D773" t="s">
+        <v>1107</v>
+      </c>
     </row>
     <row r="774" spans="1:6">
       <c r="A774" t="s">
         <v>772</v>
       </c>
+      <c r="D774" t="s">
+        <v>1013</v>
+      </c>
     </row>
     <row r="775" spans="1:6">
       <c r="A775" t="s">
         <v>773</v>
       </c>
+      <c r="D775" t="s">
+        <v>1106</v>
+      </c>
     </row>
     <row r="776" spans="1:6">
       <c r="A776" t="s">
@@ -8575,6 +9375,9 @@
       <c r="A778" t="s">
         <v>776</v>
       </c>
+      <c r="D778" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="779" spans="1:6">
       <c r="A779" t="s">
@@ -8606,22 +9409,36 @@
         <v>782</v>
       </c>
       <c r="D784" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="785" spans="1:1">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="785" spans="1:6">
       <c r="A785" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="786" spans="1:1">
+    <row r="786" spans="1:6">
       <c r="A786" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="787" spans="1:1">
+      <c r="F786" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="787" spans="1:6">
       <c r="A787" t="s">
         <v>785</v>
+      </c>
+      <c r="F787" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="788" spans="1:6">
+      <c r="A788" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D788" t="s">
+        <v>1104</v>
       </c>
     </row>
   </sheetData>
@@ -8630,103 +9447,135 @@
     <hyperlink ref="A154" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="A142" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="A143" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A144" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A146" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C146" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A152" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A385" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C383" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C384" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C387" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C388" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A419" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A418" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B418" r:id="rId16" display="http://www.lygeros.org/0052-fr.html" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A283" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B187" r:id="rId18" display="http://perso.orange.fr/therese.eveilleau/pages/truc_mat/pythagor/textes/triangles-chinois.htm" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D131" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B131" r:id="rId20" display="http://math.stanford.edu/~rhoades/FILES/setpartitions.pdf" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B132" r:id="rId21" display="http://math.stanford.edu/~rhoades/FILES/unimodal.pdf" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B82" r:id="rId22" display="http://groups.google.com/group/sumprimes/web/sumtwinsfirstn-c" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B84" r:id="rId23" display="http://hdl.handle.net/10515/sy5ft8f01" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B85" r:id="rId24" display="http://hdl.handle.net/10515/sy5sj1b71" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B86" r:id="rId25" display="http://hdl.handle.net/1773/26116" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B87" r:id="rId26" display="http://hdl.handle.net/1850/2773" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B47" r:id="rId27" display="http://dx.doi.org/10.1002/zamm.19620421310" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B48" r:id="rId28" display="http://dx.doi.org/10.1007/BF0255954" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B49" r:id="rId29" display="http://dx.doi.org/10.1007/BF02837121" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B50" r:id="rId30" display="http://dx.doi.org/10.1007/s108-01-005-4531-6" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C51" r:id="rId31" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B52" r:id="rId32" display="http://dx.doi.org/10.1016/0095-8856(79)90070-4" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B51" r:id="rId33" display="http://dx.doi.org/10.1016/0012-365X(76)90009-1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C52" r:id="rId34" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B53" r:id="rId35" display="http://dx.doi.org/10.1080/10586458.2016.115518" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C53" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B54" r:id="rId37" display="http://dx.doi.org/10.2298/AADM120108002" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B55" r:id="rId38" display="http://dx.doi.org/10.4172/1736-4337.1000227" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B56" r:id="rId39" display="http://dx.doi.org/10.5829/idosi.mejsr.2013.13.mae.9991" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B45" r:id="rId40" display="http://dx.doi.org/:10.1016/S0012-365X(97)00189-1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C45" r:id="rId41" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B11" r:id="rId42" display="http://arxiv.org/abs/0512548" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B12" r:id="rId43" display="http://arxiv.org/abs/cond-mat/?0111169" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B13" r:id="rId44" display="http://arxiv.org/bsa/1408.1702" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A18" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B33" r:id="rId46" display="http://commons.wikimedia.org/wiki/Image:A31.gif" xr:uid="{6A97FD8D-CE02-430C-8766-DEF677EA6FFB}"/>
-    <hyperlink ref="C43" r:id="rId47" tooltip="Persistent link using digital object identifier" xr:uid="{47E9B973-B6D5-422B-9F0E-8135BAADE0F6}"/>
-    <hyperlink ref="C195" r:id="rId48" xr:uid="{B288F65E-D54D-4A23-8706-673163B29C7F}"/>
-    <hyperlink ref="C196" r:id="rId49" xr:uid="{FEBA0D7B-4B03-403C-8373-04C8D24A3058}"/>
-    <hyperlink ref="C197" r:id="rId50" xr:uid="{B9913139-B4DE-47EB-A52E-52E34AAB295B}"/>
-    <hyperlink ref="C198" r:id="rId51" xr:uid="{ADEEDD12-98F0-47C7-A13C-D6989E742007}"/>
-    <hyperlink ref="C199" r:id="rId52" xr:uid="{AA43E3EC-2B7C-48B0-86E0-48F4EEC45626}"/>
-    <hyperlink ref="C200" r:id="rId53" xr:uid="{5FFFD5D6-F54E-4BAE-98E6-E07E70D8D04D}"/>
-    <hyperlink ref="C218" r:id="rId54" xr:uid="{4354FC88-D712-4707-A9C7-01336A75F185}"/>
-    <hyperlink ref="C217" r:id="rId55" xr:uid="{D6D0EA6F-7C97-411E-BFCD-6B3643F1B3C5}"/>
-    <hyperlink ref="C216" r:id="rId56" xr:uid="{99AF5E14-68B6-493A-A72F-6981DCA82946}"/>
-    <hyperlink ref="C214" r:id="rId57" xr:uid="{46272C16-B4AD-4348-BA52-CE83D1C29486}"/>
-    <hyperlink ref="C213" r:id="rId58" xr:uid="{C9712B0F-D3B9-4E6A-AC46-C7E407AC22B4}"/>
-    <hyperlink ref="C212" r:id="rId59" xr:uid="{064769B1-5B7F-4AFA-AAB5-72A4B297D917}"/>
-    <hyperlink ref="C209" r:id="rId60" xr:uid="{DC1CEEAC-FC6A-4C90-87A4-5D325148CF76}"/>
-    <hyperlink ref="C208" r:id="rId61" xr:uid="{53018170-63F6-43B7-B5D3-EF3FAB95013C}"/>
-    <hyperlink ref="C207" r:id="rId62" xr:uid="{DC7032A8-481E-4FA5-A19A-26D1AC467940}"/>
-    <hyperlink ref="C206" r:id="rId63" xr:uid="{3C0DF094-A103-4308-A578-4AC0EC79E065}"/>
-    <hyperlink ref="C205" r:id="rId64" xr:uid="{6547EFED-A006-4847-8899-62AD3640EF3C}"/>
-    <hyperlink ref="C204" r:id="rId65" xr:uid="{DC436989-A134-4073-883A-64361D5DF8B0}"/>
-    <hyperlink ref="B220" r:id="rId66" display="http://projecteuclid.org/getRecord?id=euclid.pjm/1103043674" xr:uid="{5BEDA7FA-8250-47FB-9E78-5111EF22F967}"/>
-    <hyperlink ref="B275" r:id="rId67" display="http://www.carma.newcastle.edu.au/~jb616/DR_MatrixCompletion.pdf" xr:uid="{1DEA78D3-9840-487C-9332-0645B7EE53B9}"/>
-    <hyperlink ref="C275" r:id="rId68" xr:uid="{30D44264-3C90-4E1B-B7E6-770BAAB45FCD}"/>
-    <hyperlink ref="C276" r:id="rId69" xr:uid="{4437BEC2-7567-495A-8B34-1C6F588A0369}"/>
-    <hyperlink ref="C277" r:id="rId70" xr:uid="{721BEAEB-B711-4FD8-A177-AD97AD556328}"/>
-    <hyperlink ref="C278" r:id="rId71" xr:uid="{218C405E-0B34-4E32-B43C-0189A1E493DC}"/>
-    <hyperlink ref="B299" r:id="rId72" display="http://www.combinatorics.cn/activities/notes.pdf" xr:uid="{C64331BB-716A-4BA8-8BED-37D431C46042}"/>
-    <hyperlink ref="B300" r:id="rId73" display="http://www.combinatorics.cn/publications/papers/2004/Triangle.pdf" xr:uid="{0D072083-1A40-4090-B6D9-1F3D4654574F}"/>
-    <hyperlink ref="B325" r:id="rId74" display="http://www.dmtcs.org/dmtcs-ojs/index.php/dmtcs/article/viewArticle/1334" xr:uid="{6C805ACE-A971-4786-861D-9ADB0A97AC0F}"/>
-    <hyperlink ref="B327" r:id="rId75" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewArticle/dmAJ0115" xr:uid="{D2F002A0-7390-492F-BDD2-3E06261518DD}"/>
-    <hyperlink ref="B328" r:id="rId76" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewFile/dmAT0130/4488" xr:uid="{FCE6D53A-DB36-4BC2-843C-461FCCFF8354}"/>
-    <hyperlink ref="B329" r:id="rId77" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewFile/dmAT0159/4536" xr:uid="{49E39D39-00B2-4DD4-8FB3-CE7D3E614ED1}"/>
-    <hyperlink ref="B330" r:id="rId78" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewFile/dmAT0159/4546" xr:uid="{9B52C56B-96EC-4866-A9B6-4CF38D8FA848}"/>
-    <hyperlink ref="B331" r:id="rId79" display="http://www.dmtcs.org/volumes/abstracts/dm030402.abs.html" xr:uid="{AC9082B2-EAD5-47BF-B58F-A7C0C92483A4}"/>
-    <hyperlink ref="B332" r:id="rId80" display="http://www.dmtcs.org/volumes/abstracts/dm040103.abs.html" xr:uid="{49F540C9-C61B-4B7E-8388-3CFEFDEBFBC2}"/>
-    <hyperlink ref="B7" r:id="rId81" display="http://pollack.uga.edu/mullin.pdf" xr:uid="{A9F5A3A7-110C-41D0-9455-916432A8CB21}"/>
-    <hyperlink ref="B8" r:id="rId82" display="http://alpha.math.uga.edu/~pollack/multpart.pdf" xr:uid="{413958BD-42D2-433C-AA24-5B2FE9C88356}"/>
-    <hyperlink ref="B9" r:id="rId83" display="http://alpha.math.uga.edu/~pollack/reversal12.pdf" xr:uid="{1AA4A45F-CD4E-451A-B48F-7BA2C7D2DEFE}"/>
-    <hyperlink ref="B10" r:id="rId84" display="http://alpha.math.uga.edu/~pollack/variations.pdf" xr:uid="{FE99169D-130A-48DD-9C21-EF9DF47A1DCE}"/>
-    <hyperlink ref="B6" r:id="rId85" display="http://alpha.math.uga.edu/~pollack/INTEGERS2013.pdf" xr:uid="{809F9D9B-F8E2-4654-BBAB-66A24D999F1C}"/>
-    <hyperlink ref="B367" r:id="rId86" display="http://www.hindawi.com/GetArticle.aspx?doi=10.1155/S0161171295000512" xr:uid="{65C631F7-9B14-46CB-AAE1-6B5C88905165}"/>
-    <hyperlink ref="B478" r:id="rId87" display="http://www.math.ualberta.ca/~subbarao/documents/2002_Pillai.pdf" xr:uid="{B8CC0AAE-864E-4CD5-925C-953D649CDB18}"/>
-    <hyperlink ref="C513" r:id="rId88" xr:uid="{0DA9818A-BFE3-4892-B5FF-708D1BCEA426}"/>
-    <hyperlink ref="C514" r:id="rId89" xr:uid="{BA5C8B0A-AE97-40FC-92C3-DCDBF764CB86}"/>
-    <hyperlink ref="C515" r:id="rId90" xr:uid="{EA69507E-6954-4FDA-B341-47438E70820E}"/>
-    <hyperlink ref="C655" r:id="rId91" xr:uid="{840F3F91-A5AA-4C06-BFDB-FBDE6BC99DCC}"/>
-    <hyperlink ref="C656" r:id="rId92" xr:uid="{AED51E0E-AA3E-4934-A4A5-DAA0D28F35AF}"/>
-    <hyperlink ref="C657" r:id="rId93" xr:uid="{3FCA5E5E-6C01-48C8-88DE-1B037E72094F}"/>
-    <hyperlink ref="C658" r:id="rId94" xr:uid="{8BDF7D53-4D71-4E25-BF4A-32BDA72BECAA}"/>
-    <hyperlink ref="C659" r:id="rId95" xr:uid="{2BB3453F-DA52-4374-8D84-1F0B5DF7C3C3}"/>
-    <hyperlink ref="C660" r:id="rId96" xr:uid="{320A7D17-EA4A-4CDC-8D25-523F608150DB}"/>
+    <hyperlink ref="A146" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C146" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A152" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A385" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C383" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C384" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C387" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C388" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A419" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A418" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B418" r:id="rId15" display="http://www.lygeros.org/0052-fr.html" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A283" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B187" r:id="rId17" display="http://perso.orange.fr/therese.eveilleau/pages/truc_mat/pythagor/textes/triangles-chinois.htm" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D131" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B131" r:id="rId19" display="http://math.stanford.edu/~rhoades/FILES/setpartitions.pdf" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B132" r:id="rId20" display="http://math.stanford.edu/~rhoades/FILES/unimodal.pdf" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B82" r:id="rId21" display="http://groups.google.com/group/sumprimes/web/sumtwinsfirstn-c" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B84" r:id="rId22" display="http://hdl.handle.net/10515/sy5ft8f01" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B85" r:id="rId23" display="http://hdl.handle.net/10515/sy5sj1b71" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B86" r:id="rId24" display="http://hdl.handle.net/1773/26116" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B87" r:id="rId25" display="http://hdl.handle.net/1850/2773" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B47" r:id="rId26" display="http://dx.doi.org/10.1002/zamm.19620421310" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B48" r:id="rId27" display="http://dx.doi.org/10.1007/BF0255954" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B49" r:id="rId28" display="http://dx.doi.org/10.1007/BF02837121" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B50" r:id="rId29" display="http://dx.doi.org/10.1007/s108-01-005-4531-6" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C51" r:id="rId30" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B52" r:id="rId31" display="http://dx.doi.org/10.1016/0095-8856(79)90070-4" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B51" r:id="rId32" display="http://dx.doi.org/10.1016/0012-365X(76)90009-1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C52" r:id="rId33" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B53" r:id="rId34" display="http://dx.doi.org/10.1080/10586458.2016.115518" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C53" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B54" r:id="rId36" display="http://dx.doi.org/10.2298/AADM120108002" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B55" r:id="rId37" display="http://dx.doi.org/10.4172/1736-4337.1000227" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B56" r:id="rId38" display="http://dx.doi.org/10.5829/idosi.mejsr.2013.13.mae.9991" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B45" r:id="rId39" display="http://dx.doi.org/:10.1016/S0012-365X(97)00189-1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C45" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B11" r:id="rId41" display="http://arxiv.org/abs/0512548" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B12" r:id="rId42" display="http://arxiv.org/abs/cond-mat/?0111169" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B13" r:id="rId43" display="http://arxiv.org/bsa/1408.1702" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A18" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B33" r:id="rId45" display="http://commons.wikimedia.org/wiki/Image:A31.gif" xr:uid="{6A97FD8D-CE02-430C-8766-DEF677EA6FFB}"/>
+    <hyperlink ref="C43" r:id="rId46" tooltip="Persistent link using digital object identifier" xr:uid="{47E9B973-B6D5-422B-9F0E-8135BAADE0F6}"/>
+    <hyperlink ref="C195" r:id="rId47" xr:uid="{B288F65E-D54D-4A23-8706-673163B29C7F}"/>
+    <hyperlink ref="C196" r:id="rId48" xr:uid="{FEBA0D7B-4B03-403C-8373-04C8D24A3058}"/>
+    <hyperlink ref="C197" r:id="rId49" xr:uid="{B9913139-B4DE-47EB-A52E-52E34AAB295B}"/>
+    <hyperlink ref="C198" r:id="rId50" xr:uid="{ADEEDD12-98F0-47C7-A13C-D6989E742007}"/>
+    <hyperlink ref="C199" r:id="rId51" xr:uid="{AA43E3EC-2B7C-48B0-86E0-48F4EEC45626}"/>
+    <hyperlink ref="C200" r:id="rId52" xr:uid="{5FFFD5D6-F54E-4BAE-98E6-E07E70D8D04D}"/>
+    <hyperlink ref="C218" r:id="rId53" xr:uid="{4354FC88-D712-4707-A9C7-01336A75F185}"/>
+    <hyperlink ref="C217" r:id="rId54" xr:uid="{D6D0EA6F-7C97-411E-BFCD-6B3643F1B3C5}"/>
+    <hyperlink ref="C216" r:id="rId55" xr:uid="{99AF5E14-68B6-493A-A72F-6981DCA82946}"/>
+    <hyperlink ref="C214" r:id="rId56" xr:uid="{46272C16-B4AD-4348-BA52-CE83D1C29486}"/>
+    <hyperlink ref="C213" r:id="rId57" xr:uid="{C9712B0F-D3B9-4E6A-AC46-C7E407AC22B4}"/>
+    <hyperlink ref="C212" r:id="rId58" xr:uid="{064769B1-5B7F-4AFA-AAB5-72A4B297D917}"/>
+    <hyperlink ref="C209" r:id="rId59" xr:uid="{DC1CEEAC-FC6A-4C90-87A4-5D325148CF76}"/>
+    <hyperlink ref="C208" r:id="rId60" xr:uid="{53018170-63F6-43B7-B5D3-EF3FAB95013C}"/>
+    <hyperlink ref="C207" r:id="rId61" xr:uid="{DC7032A8-481E-4FA5-A19A-26D1AC467940}"/>
+    <hyperlink ref="C206" r:id="rId62" xr:uid="{3C0DF094-A103-4308-A578-4AC0EC79E065}"/>
+    <hyperlink ref="C205" r:id="rId63" xr:uid="{6547EFED-A006-4847-8899-62AD3640EF3C}"/>
+    <hyperlink ref="C204" r:id="rId64" xr:uid="{DC436989-A134-4073-883A-64361D5DF8B0}"/>
+    <hyperlink ref="B220" r:id="rId65" display="http://projecteuclid.org/getRecord?id=euclid.pjm/1103043674" xr:uid="{5BEDA7FA-8250-47FB-9E78-5111EF22F967}"/>
+    <hyperlink ref="B275" r:id="rId66" display="http://www.carma.newcastle.edu.au/~jb616/DR_MatrixCompletion.pdf" xr:uid="{1DEA78D3-9840-487C-9332-0645B7EE53B9}"/>
+    <hyperlink ref="C275" r:id="rId67" xr:uid="{30D44264-3C90-4E1B-B7E6-770BAAB45FCD}"/>
+    <hyperlink ref="C276" r:id="rId68" xr:uid="{4437BEC2-7567-495A-8B34-1C6F588A0369}"/>
+    <hyperlink ref="C277" r:id="rId69" xr:uid="{721BEAEB-B711-4FD8-A177-AD97AD556328}"/>
+    <hyperlink ref="C278" r:id="rId70" xr:uid="{218C405E-0B34-4E32-B43C-0189A1E493DC}"/>
+    <hyperlink ref="B299" r:id="rId71" display="http://www.combinatorics.cn/activities/notes.pdf" xr:uid="{C64331BB-716A-4BA8-8BED-37D431C46042}"/>
+    <hyperlink ref="B300" r:id="rId72" display="http://www.combinatorics.cn/publications/papers/2004/Triangle.pdf" xr:uid="{0D072083-1A40-4090-B6D9-1F3D4654574F}"/>
+    <hyperlink ref="B325" r:id="rId73" display="http://www.dmtcs.org/dmtcs-ojs/index.php/dmtcs/article/viewArticle/1334" xr:uid="{6C805ACE-A971-4786-861D-9ADB0A97AC0F}"/>
+    <hyperlink ref="B327" r:id="rId74" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewArticle/dmAJ0115" xr:uid="{D2F002A0-7390-492F-BDD2-3E06261518DD}"/>
+    <hyperlink ref="B328" r:id="rId75" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewFile/dmAT0130/4488" xr:uid="{FCE6D53A-DB36-4BC2-843C-461FCCFF8354}"/>
+    <hyperlink ref="B329" r:id="rId76" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewFile/dmAT0159/4536" xr:uid="{49E39D39-00B2-4DD4-8FB3-CE7D3E614ED1}"/>
+    <hyperlink ref="B330" r:id="rId77" display="http://www.dmtcs.org/dmtcs-ojs/index.php/proceedings/article/viewFile/dmAT0159/4546" xr:uid="{9B52C56B-96EC-4866-A9B6-4CF38D8FA848}"/>
+    <hyperlink ref="B331" r:id="rId78" display="http://www.dmtcs.org/volumes/abstracts/dm030402.abs.html" xr:uid="{AC9082B2-EAD5-47BF-B58F-A7C0C92483A4}"/>
+    <hyperlink ref="B332" r:id="rId79" display="http://www.dmtcs.org/volumes/abstracts/dm040103.abs.html" xr:uid="{49F540C9-C61B-4B7E-8388-3CFEFDEBFBC2}"/>
+    <hyperlink ref="B7" r:id="rId80" display="http://pollack.uga.edu/mullin.pdf" xr:uid="{A9F5A3A7-110C-41D0-9455-916432A8CB21}"/>
+    <hyperlink ref="B8" r:id="rId81" display="http://alpha.math.uga.edu/~pollack/multpart.pdf" xr:uid="{413958BD-42D2-433C-AA24-5B2FE9C88356}"/>
+    <hyperlink ref="B9" r:id="rId82" display="http://alpha.math.uga.edu/~pollack/reversal12.pdf" xr:uid="{1AA4A45F-CD4E-451A-B48F-7BA2C7D2DEFE}"/>
+    <hyperlink ref="B10" r:id="rId83" display="http://alpha.math.uga.edu/~pollack/variations.pdf" xr:uid="{FE99169D-130A-48DD-9C21-EF9DF47A1DCE}"/>
+    <hyperlink ref="B6" r:id="rId84" display="http://alpha.math.uga.edu/~pollack/INTEGERS2013.pdf" xr:uid="{809F9D9B-F8E2-4654-BBAB-66A24D999F1C}"/>
+    <hyperlink ref="B367" r:id="rId85" display="http://www.hindawi.com/GetArticle.aspx?doi=10.1155/S0161171295000512" xr:uid="{65C631F7-9B14-46CB-AAE1-6B5C88905165}"/>
+    <hyperlink ref="B478" r:id="rId86" display="http://www.math.ualberta.ca/~subbarao/documents/2002_Pillai.pdf" xr:uid="{B8CC0AAE-864E-4CD5-925C-953D649CDB18}"/>
+    <hyperlink ref="C513" r:id="rId87" xr:uid="{0DA9818A-BFE3-4892-B5FF-708D1BCEA426}"/>
+    <hyperlink ref="C514" r:id="rId88" xr:uid="{BA5C8B0A-AE97-40FC-92C3-DCDBF764CB86}"/>
+    <hyperlink ref="C515" r:id="rId89" xr:uid="{EA69507E-6954-4FDA-B341-47438E70820E}"/>
+    <hyperlink ref="C655" r:id="rId90" xr:uid="{840F3F91-A5AA-4C06-BFDB-FBDE6BC99DCC}"/>
+    <hyperlink ref="C656" r:id="rId91" xr:uid="{AED51E0E-AA3E-4934-A4A5-DAA0D28F35AF}"/>
+    <hyperlink ref="C657" r:id="rId92" xr:uid="{3FCA5E5E-6C01-48C8-88DE-1B037E72094F}"/>
+    <hyperlink ref="C658" r:id="rId93" xr:uid="{8BDF7D53-4D71-4E25-BF4A-32BDA72BECAA}"/>
+    <hyperlink ref="C659" r:id="rId94" xr:uid="{2BB3453F-DA52-4374-8D84-1F0B5DF7C3C3}"/>
+    <hyperlink ref="C660" r:id="rId95" xr:uid="{320A7D17-EA4A-4CDC-8D25-523F608150DB}"/>
+    <hyperlink ref="C738" r:id="rId96" xr:uid="{6F28E8D1-D1E1-4CDA-BD84-A445E89861C8}"/>
+    <hyperlink ref="C739" r:id="rId97" xr:uid="{15E183D0-342C-4CE0-AD69-6C51C3DF60AB}"/>
+    <hyperlink ref="C740" r:id="rId98" xr:uid="{757BF2F0-D271-4282-BF49-3F95FC8E4A23}"/>
+    <hyperlink ref="C741" r:id="rId99" xr:uid="{CA2AC94E-CCFE-46AB-B90D-C75727800B81}"/>
+    <hyperlink ref="C742" r:id="rId100" xr:uid="{FC9D7945-752B-4763-B0AB-5AD7F45C5AC6}"/>
+    <hyperlink ref="C25" r:id="rId101" xr:uid="{088C6741-C462-4286-ADC4-7A67AEE7542C}"/>
+    <hyperlink ref="A144" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId103" display="http://atlas-conferences.com/cgi-bin/abstract/cbbv-77" xr:uid="{2261BEC0-445F-4EC5-8AD6-4D98DED300EF}"/>
+    <hyperlink ref="B72" r:id="rId104" display="http://fpsac.labri.fr/FPSAC97/articles.html" xr:uid="{898579AD-9C86-4CC3-973C-C3FAC22A1649}"/>
+    <hyperlink ref="C72" r:id="rId105" tooltip="Persistent link using digital object identifier" xr:uid="{FC402196-6B43-4813-8B3A-36525BEAE317}"/>
+    <hyperlink ref="A93" r:id="rId106" xr:uid="{855C5188-2491-452E-A742-8FDC38822F49}"/>
+    <hyperlink ref="A108" r:id="rId107" xr:uid="{1EFCCE71-19C9-4F79-B215-4792B78518E0}"/>
+    <hyperlink ref="C118" r:id="rId108" xr:uid="{EEDD3862-6DDC-4248-A909-17A66C314735}"/>
+    <hyperlink ref="C117" r:id="rId109" xr:uid="{4C7A306C-BDE8-4260-B9EA-A73E2E841C0C}"/>
+    <hyperlink ref="B121" r:id="rId110" display="http://math.nju.edu.cn/~zwsun/139d.pdf" xr:uid="{B0D8B0C9-6136-4C29-A759-927E0A13CF01}"/>
+    <hyperlink ref="D123" r:id="rId111" tooltip="Persistent link using digital object identifier" xr:uid="{B9EDAF8E-35D8-47BE-961E-FF13AF4C34EE}"/>
+    <hyperlink ref="B127" r:id="rId112" display="http://math.rice.edu/~lanius/frac/koch/koch.html" xr:uid="{5A05A8A2-9F2D-4308-A3C2-77BC5BBCCD14}"/>
+    <hyperlink ref="B134" r:id="rId113" display="http://math.uark.edu/Eastwood5.pdf" xr:uid="{E2E37801-6629-4EB3-BD3C-AAD5D707FA4A}"/>
+    <hyperlink ref="B305" r:id="rId114" display="http://www.cs.arizona.edu/patterns/sequences.html" xr:uid="{E7689E69-E480-4FCC-AAA8-4A51DE2D4543}"/>
+    <hyperlink ref="B306" r:id="rId115" display="http://www.cs.cmu.edu/~sutner/papers/em-sequence.ps.gz" xr:uid="{AB8DB1F9-ECA9-46EF-A6A4-0BCD9DE4AC81}"/>
+    <hyperlink ref="B311" r:id="rId116" display="http://www.cs.ucl.ac.uk/staff/S.Bhatti/D51-notes/node30.html" xr:uid="{82C9C586-7498-4119-9F89-1A9A67982E12}"/>
+    <hyperlink ref="A315" r:id="rId117" xr:uid="{1E3782D1-F9A6-4ED8-AAE3-483BD4A16EAB}"/>
+    <hyperlink ref="B312" r:id="rId118" display="http://www.cs.utexas.edu/users/s2s/latest/viskoch1/src/visualKoch.htm" xr:uid="{85A4E15B-6999-4D8C-8A37-C55040A657AA}"/>
+    <hyperlink ref="B310" r:id="rId119" display="http://www.cs.toronto.edu/~mackay/sumsquares.pdf" xr:uid="{90886036-F7A4-4F5F-B30E-A29EDB21C7E0}"/>
+    <hyperlink ref="B336" r:id="rId120" display="http://www.dsi.dsi.unifi.it/~resp/GouldBK.pdf" xr:uid="{475B6D9F-507B-4394-9EF0-CAB31E2ECADB}"/>
+    <hyperlink ref="B338" r:id="rId121" display="http://www.dsi.unifi.it/~resp/GouldBK.pdf" xr:uid="{38DC02C9-A451-4765-B412-5A2C764E3378}"/>
+    <hyperlink ref="B339" r:id="rId122" display="http://www.ece.uvic.ca/~agullive/square.ps" xr:uid="{1D396DD7-15AF-46E4-BA25-6EBEAECC8DE6}"/>
+    <hyperlink ref="B347" r:id="rId123" display="http://www.exp-math.uni-essen.de/~immink/pdf/jsac13.pdf" xr:uid="{778903BD-E2CE-477D-B85F-E7CF13E1138A}"/>
+    <hyperlink ref="B359" r:id="rId124" location="Gematria" display="http://www.geocities.com/Athens/Oracle/4581/hebintro.html - Gematria" xr:uid="{97212397-5D76-42CB-816C-03652907D6A0}"/>
+    <hyperlink ref="A675" r:id="rId125" xr:uid="{04CF27F5-B4E7-40B2-A365-8B8880E60B95}"/>
+    <hyperlink ref="C752" r:id="rId126" xr:uid="{85B3017C-57A5-4315-8634-50A155E99DBA}"/>
+    <hyperlink ref="A614" r:id="rId127" xr:uid="{BE4A11B8-840F-4E92-B887-31ACA717F219}"/>
+    <hyperlink ref="B757" r:id="rId128" display="https://doi.org/10.18311/jims/1942/17182" xr:uid="{6896B2FF-215B-424F-8E91-DAF3FB5B8026}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId97"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId129"/>
   <tableParts count="1">
-    <tablePart r:id="rId98"/>
+    <tablePart r:id="rId130"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Another batch of links fixed
</commit_message>
<xml_diff>
--- a/broken.xlsx
+++ b/broken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01028734c1c2e442/Рабочий стол/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="416" documentId="13_ncr:40009_{750DEEBC-8306-47E1-A9AD-D352C13D1A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{601FEC47-6FD4-451E-8F68-0E69BA45EA15}"/>
+  <xr:revisionPtr revIDLastSave="572" documentId="13_ncr:40009_{750DEEBC-8306-47E1-A9AD-D352C13D1A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8EAF5AEB-8204-409B-961E-392E903F94DE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="1197">
   <si>
     <t>http://14142.net/n-puzzle/document/document.html</t>
   </si>
@@ -2281,9 +2281,6 @@
     <t>https://doi.org/10.114/S1793042120500475</t>
   </si>
   <si>
-    <t>https://doi.org/10.1387/ekaia.17851</t>
-  </si>
-  <si>
     <t>https://doi.org/10.15330/cmp.12.1.10-18</t>
   </si>
   <si>
@@ -3374,6 +3371,246 @@
   </si>
   <si>
     <t>https://www.ejournals.eu/sj/index.php/SI/article/view/2227</t>
+  </si>
+  <si>
+    <t>National Institute of Standards and Technology, Hamming distance</t>
+  </si>
+  <si>
+    <t>https://www.nobelprize.org/prizes/chemistry/1922/aston/lecture/</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/On-Some-Functions-Involving-the-lcm-and-gcd-of-Bagdasar/467a76bae8688870407d9b6d7ef0679bbbfcf797</t>
+  </si>
+  <si>
+    <t>https://www.math.uni-bielefeld.de/~sillke/PUZZLES/quantum/bridgarc.html</t>
+  </si>
+  <si>
+    <t>https://www.cs.hmc.edu/ACM/Problems/Fall00/jugfill/jugfill.html</t>
+  </si>
+  <si>
+    <t>http://www.numdam.org/article/PMIHES_1981__53__53_0.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elizabeth Wilmer, Notes on Stephan's conjectures 72, 73 and 74 </t>
+  </si>
+  <si>
+    <t>http://citeseerx.ist.psu.edu/viewdoc/download?doi=10.1.1.210.3627&amp;rep=rep1&amp;type=pdf</t>
+  </si>
+  <si>
+    <t>David Rock, Problem of the Week</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20120314005924/http://www.ortelius.de/kalender/east_en.php</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20170407203826/http://www.mathsolympiad.org.nz/wp-content/uploads/2009/01/bertrands-theorem.pdf</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20071123155400/http://www.maths.gla.ac.uk/~es/hadamard.html</t>
+  </si>
+  <si>
+    <t>https://www.mathpages.com/home/kmath477/kmath477.htm</t>
+  </si>
+  <si>
+    <t>https://www.mathpages.com/home/kmath381/kmath381.htm</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/0903.3026</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1515/dema-2013-0418</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/On-multi-avoidance-of-right-angled-numbered-Kitaev/a51353d11ab14dd4b69026e2ed1e1f97efe465ee</t>
+  </si>
+  <si>
+    <t>http://www.pentadecathlon.com/objects/class1/class1.php</t>
+  </si>
+  <si>
+    <t>https://www.pbs.org/wgbh/nova/article/plancks-constant/</t>
+  </si>
+  <si>
+    <t>http://www2.math.uu.se/~svante/papers/sj114.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1137/S036301299325270X</t>
+  </si>
+  <si>
+    <t>http://www.njohnston.ca/2009/05/on-maximal-self-avoiding-walks/</t>
+  </si>
+  <si>
+    <t>http://match.pmf.kg.ac.rs/electronic_versions/Match68/n1/match68n1_31-64.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2298/FIL1510207M</t>
+  </si>
+  <si>
+    <t>https://www.primepuzzles.net/puzzles/puzz_270.htm</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20150412114922/http://www.problem-solving.be/pen/published/pen-20070711.pdf</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20140607165152/http://www.prooffreader.com/2014/05/graphing-distribution-of-english.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20170107132755/http://www.qucosa.de/fileadmin/data/qucosa/documents/10115/DissertationFrankSimon.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/math/0311235</t>
+  </si>
+  <si>
+    <t>Amotz Bar-Noy, Graph Algorithms, Chromatic Polynomials</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20180417043918/http://www.sci.brooklyn.cuny.edu/~amotz/GC-ALGORITHMS/PRESENTATIONS/chromatic.pdf</t>
+  </si>
+  <si>
+    <t>The Nine Planets, Perfect Numbers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/00029890.2006.11920376</t>
+  </si>
+  <si>
+    <t>https://archive.bridgesmathart.org/2004/bridges2004-189.html</t>
+  </si>
+  <si>
+    <t>Skidmore College Problem Group, Solution to Problem #913 from the Pi Mu Epsilon Journal</t>
+  </si>
+  <si>
+    <t>Schneider, Joel, et al., Mathnet Guide</t>
+  </si>
+  <si>
+    <t>T. Granlund, Repunits.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1090/S0025-5718-08-02166-2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/18.651069</t>
+  </si>
+  <si>
+    <t>Viswanathan Anand, The Indian Defense, Time, Jun 19 2008</t>
+  </si>
+  <si>
+    <t>http://tkmh.space/assets/files/pisano_semiperiod.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tower Records, Beethoven's 5th symphony </t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/Principles-of-Symmetry%2C-Dynamics%2C-and-Spectroscopy-Harter-Judd/b150be8165c61e1b1b3852787192606e9d7070f8</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/0708.0809</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20080315204129/http://www.unc.edu/~rowlett/units/scales/beaufort.html</t>
+  </si>
+  <si>
+    <t>H. Fripertinger, The Euler phi function</t>
+  </si>
+  <si>
+    <t>E. G. Richards, Mapping Time, The Calendar and its History, Oxford University Press, Great Clarendon Street, Oxford OX2 6DP, Reprinted 1999 (with corrections) page 231-5, 290, 311, 321.</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/mappingtimecalen00rich</t>
+  </si>
+  <si>
+    <t>https://ericmoorhouse.org/pub/planes/</t>
+  </si>
+  <si>
+    <t>https://washingtonart.net/whealton/PFCN.html</t>
+  </si>
+  <si>
+    <t>A. Weimholt, 16-cell net</t>
+  </si>
+  <si>
+    <t>Marcus Jaiclin, Pascal's Triangle, Mod 2,3,5</t>
+  </si>
+  <si>
+    <t>https://projecteuclid.org/euclid.involve/1513733722</t>
+  </si>
+  <si>
+    <t>http://people.reed.edu/~davidp/homepage/students/alt.pdf</t>
+  </si>
+  <si>
+    <t>https://wyattalt.com/files/thesis.pdf</t>
+  </si>
+  <si>
+    <t>needs a large edit</t>
+  </si>
+  <si>
+    <t>D. R. Herrick, Home Page</t>
+  </si>
+  <si>
+    <t>J. Pan, Multiple Binomial Transforms and Families of Integer Sequences , J. Int. Seq. 13 (2010), 10.4.2, T^(2).</t>
+  </si>
+  <si>
+    <t>https://cs.uwaterloo.ca/journals/JIS/VOL13/Pan/pan8.pdf</t>
+  </si>
+  <si>
+    <t>https://cs.uwaterloo.ca/journals/JIS/VOL7/Moree/moree12.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/0022-314X%2888%2990093-5</t>
+  </si>
+  <si>
+    <t>Benoit Cloitre, Graph of (sum(k=6,n,a(k))-2n)*n^(-1/2), pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/kolosovpetro/Mathematica-scripts/tree/master/arxiv1603.02468</t>
+  </si>
+  <si>
+    <t>Achilles A. Beros, Bjørn Kjos-Hanssen, Daylan Kaui, The number of long words having a given automatic complexity*, 2018.</t>
+  </si>
+  <si>
+    <t>Zhi-Wei Sun, Write 2n+1 &gt; 14 as p+q+r with p,q,r odd primes and 2p+4q+6r a square, Question 331170 on MathOverflow, May 10, 2019.</t>
+  </si>
+  <si>
+    <t>https://oam-rc.inoe.ro/articles/on-atom-bond-connectivity-and-ga-indices-of-nanocones/fulltext</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/FURTHER-COMBINATORIAL-PROPERTIES-OF-THE-SYMMETRIC-Laradji-Umar/0c18382dcbcacc5c3a7d828ee2b94951c9500cc9</t>
+  </si>
+  <si>
+    <t>H. U. Besche, B. Eick and E. A. O'Brien, Number of isomorphism types of finite groups of given order</t>
+  </si>
+  <si>
+    <t>H. U. Besche, B. Eick, and E. A. O'Brien, The SmallGroups Library - a library of groups of small order, 2005, an accepted and refereed GAP package, available also in MAGMA.</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/Complete-combinatorial-generation-of-small-point-Finschi-Fukuda/928e544c951675b69b1f54b9c0b3fc18a1c6efdd</t>
+  </si>
+  <si>
+    <t>M. Wolf, On Twin and Cousin Primes</t>
+  </si>
+  <si>
+    <t>https://www.semanticscholar.org/paper/On-the-Twin-and-Cousin-Primes-Wolf/efa69289aa31f0260e0b603e951b0e25bd875fae</t>
+  </si>
+  <si>
+    <t>William P. Orrick, Spectrum of the determinant function</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/0012-365x(93)e0230-2</t>
+  </si>
+  <si>
+    <t>Mitch Hight, United States Coinage History</t>
+  </si>
+  <si>
+    <t>M. S. Waterman, Home Page</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1006/jcta.1997.2846</t>
+  </si>
+  <si>
+    <t>I. V. Serov, CHF Diatomic Algorithm Benchmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R. G. E. Pinch, Economical numbers. </t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/math/9802046</t>
   </si>
 </sst>
 </file>
@@ -4275,10 +4512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F788"/>
+  <dimension ref="A1:F787"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A678" sqref="A678"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4293,22 +4530,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B1" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1" t="s">
         <v>786</v>
       </c>
-      <c r="B1" t="s">
-        <v>791</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>787</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>788</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>789</v>
-      </c>
-      <c r="F1" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4321,10 +4558,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4332,7 +4569,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4345,13 +4582,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C6" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4359,10 +4596,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C7" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4370,13 +4607,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C8" t="s">
         <v>958</v>
       </c>
-      <c r="C8" t="s">
-        <v>959</v>
-      </c>
       <c r="F8" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4384,10 +4621,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4395,13 +4632,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C10" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F10" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4409,13 +4646,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C11" t="s">
         <v>866</v>
       </c>
-      <c r="C11" t="s">
-        <v>867</v>
-      </c>
       <c r="F11" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -4423,13 +4660,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C12" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F12" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4437,13 +4674,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C13" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F13" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4451,10 +4688,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F14" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4482,7 +4719,7 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4505,7 +4742,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4513,7 +4750,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4521,7 +4758,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4559,10 +4796,10 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F32" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4570,7 +4807,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4603,10 +4840,10 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F39" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -4629,7 +4866,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -4642,13 +4879,13 @@
         <v>54</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>865</v>
-      </c>
       <c r="F45" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4656,7 +4893,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4664,7 +4901,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4672,10 +4909,10 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D48" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -4683,7 +4920,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -4691,10 +4928,10 @@
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="D50" t="s">
         <v>850</v>
-      </c>
-      <c r="D50" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -4702,10 +4939,10 @@
         <v>48</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -4713,10 +4950,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -4724,10 +4961,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>856</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -4735,10 +4972,10 @@
         <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="D54" t="s">
         <v>858</v>
-      </c>
-      <c r="D54" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -4746,10 +4983,10 @@
         <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D55" t="s">
         <v>860</v>
-      </c>
-      <c r="D55" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -4757,10 +4994,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D56" t="s">
         <v>862</v>
-      </c>
-      <c r="D56" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -4793,7 +5030,7 @@
         <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -4846,13 +5083,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>1045</v>
-      </c>
       <c r="F72" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4905,7 +5142,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4918,13 +5155,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D84" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F84" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -4932,10 +5169,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D85" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -4943,10 +5180,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -4954,13 +5191,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F87" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -4986,7 +5223,7 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D91" s="4"/>
     </row>
@@ -5013,7 +5250,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -5031,7 +5268,7 @@
         <v>96</v>
       </c>
       <c r="D98" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -5039,7 +5276,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -5047,7 +5284,7 @@
         <v>98</v>
       </c>
       <c r="D100" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -5055,7 +5292,7 @@
         <v>99</v>
       </c>
       <c r="D101" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -5083,7 +5320,7 @@
         <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -5091,7 +5328,7 @@
         <v>105</v>
       </c>
       <c r="D107" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -5109,7 +5346,7 @@
         <v>108</v>
       </c>
       <c r="D110" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -5127,7 +5364,7 @@
         <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -5150,7 +5387,7 @@
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -5158,7 +5395,7 @@
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -5176,10 +5413,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D121" t="s">
         <v>1058</v>
-      </c>
-      <c r="D121" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -5187,7 +5424,7 @@
         <v>121</v>
       </c>
       <c r="D122" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -5195,7 +5432,7 @@
         <v>122</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -5203,7 +5440,7 @@
         <v>123</v>
       </c>
       <c r="D124" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -5211,7 +5448,7 @@
         <v>124</v>
       </c>
       <c r="D125" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -5219,7 +5456,7 @@
         <v>125</v>
       </c>
       <c r="D126" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -5227,7 +5464,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -5240,7 +5477,7 @@
         <v>128</v>
       </c>
       <c r="D129" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -5248,7 +5485,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -5256,10 +5493,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -5267,7 +5504,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -5275,7 +5512,7 @@
         <v>115</v>
       </c>
       <c r="D133" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -5283,10 +5520,10 @@
         <v>132</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D134" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -5329,7 +5566,7 @@
         <v>140</v>
       </c>
       <c r="C142" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -5337,7 +5574,7 @@
         <v>141</v>
       </c>
       <c r="C143" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -5345,7 +5582,7 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -5353,7 +5590,7 @@
         <v>143</v>
       </c>
       <c r="C145" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -5361,7 +5598,7 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -5369,7 +5606,7 @@
         <v>154</v>
       </c>
       <c r="C147" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -5377,7 +5614,7 @@
         <v>145</v>
       </c>
       <c r="C148" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5385,10 +5622,10 @@
         <v>146</v>
       </c>
       <c r="C149" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F149" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -5396,7 +5633,7 @@
         <v>147</v>
       </c>
       <c r="C150" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -5404,7 +5641,7 @@
         <v>148</v>
       </c>
       <c r="C151" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -5412,7 +5649,7 @@
         <v>149</v>
       </c>
       <c r="C152" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -5420,7 +5657,7 @@
         <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -5428,7 +5665,7 @@
         <v>150</v>
       </c>
       <c r="B154" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -5436,7 +5673,7 @@
         <v>151</v>
       </c>
       <c r="C155" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -5444,7 +5681,7 @@
         <v>152</v>
       </c>
       <c r="C156" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -5452,7 +5689,7 @@
         <v>153</v>
       </c>
       <c r="C157" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -5595,10 +5832,10 @@
         <v>183</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C185" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -5606,7 +5843,7 @@
         <v>184</v>
       </c>
       <c r="C186" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -5614,7 +5851,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5622,7 +5859,7 @@
         <v>186</v>
       </c>
       <c r="C188" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -5630,10 +5867,10 @@
         <v>187</v>
       </c>
       <c r="C189" t="s">
+        <v>825</v>
+      </c>
+      <c r="F189" t="s">
         <v>826</v>
-      </c>
-      <c r="F189" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -5641,7 +5878,7 @@
         <v>188</v>
       </c>
       <c r="C190" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -5649,7 +5886,7 @@
         <v>189</v>
       </c>
       <c r="C191" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -5672,7 +5909,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -5680,7 +5917,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -5688,7 +5925,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -5696,7 +5933,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -5704,7 +5941,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -5712,7 +5949,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -5720,7 +5957,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -5728,7 +5965,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -5736,7 +5973,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -5744,7 +5981,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -5752,7 +5989,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -5760,7 +5997,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -5768,7 +6005,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -5776,7 +6013,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -5784,7 +6021,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -5792,7 +6029,7 @@
         <v>208</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -5800,7 +6037,7 @@
         <v>209</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -5808,7 +6045,7 @@
         <v>210</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -5816,7 +6053,7 @@
         <v>211</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -5824,7 +6061,7 @@
         <v>213</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -5832,7 +6069,7 @@
         <v>212</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -5840,7 +6077,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -5848,7 +6085,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -5856,10 +6093,10 @@
         <v>216</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F218" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -5872,13 +6109,13 @@
         <v>218</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C220" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F220" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -5951,7 +6188,7 @@
         <v>232</v>
       </c>
       <c r="E234" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -5959,7 +6196,7 @@
         <v>233</v>
       </c>
       <c r="E235" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -5967,7 +6204,7 @@
         <v>234</v>
       </c>
       <c r="E236" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -5975,7 +6212,7 @@
         <v>235</v>
       </c>
       <c r="D237" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -5983,7 +6220,7 @@
         <v>236</v>
       </c>
       <c r="D238" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -6001,7 +6238,7 @@
         <v>239</v>
       </c>
       <c r="C241" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="242" spans="1:6">
@@ -6014,7 +6251,7 @@
         <v>241</v>
       </c>
       <c r="F243" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="244" spans="1:6">
@@ -6032,7 +6269,7 @@
         <v>244</v>
       </c>
       <c r="E246" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="247" spans="1:6">
@@ -6040,10 +6277,10 @@
         <v>246</v>
       </c>
       <c r="C247" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F247" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="248" spans="1:6">
@@ -6051,7 +6288,7 @@
         <v>245</v>
       </c>
       <c r="C248" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="249" spans="1:6">
@@ -6079,7 +6316,7 @@
         <v>251</v>
       </c>
       <c r="C253" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="254" spans="1:6">
@@ -6137,7 +6374,7 @@
         <v>267</v>
       </c>
       <c r="D264" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -6195,10 +6432,10 @@
         <v>278</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>906</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -6206,7 +6443,7 @@
         <v>279</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -6214,7 +6451,7 @@
         <v>280</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -6222,7 +6459,7 @@
         <v>281</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -6240,7 +6477,7 @@
         <v>284</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -6248,7 +6485,7 @@
         <v>285</v>
       </c>
       <c r="D282" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -6271,116 +6508,137 @@
         <v>289</v>
       </c>
       <c r="B286" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
         <v>290</v>
       </c>
+      <c r="B287" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D287" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="289" spans="1:4">
+      <c r="B288" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6">
       <c r="A289" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="290" spans="1:4">
+    <row r="290" spans="1:6">
       <c r="A290" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="291" spans="1:4">
+      <c r="D290" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6">
       <c r="A291" t="s">
         <v>294</v>
       </c>
       <c r="C291" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6">
       <c r="A292" t="s">
         <v>295</v>
       </c>
       <c r="C292" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6">
       <c r="A293" t="s">
         <v>296</v>
       </c>
       <c r="C293" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6">
       <c r="A294" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="295" spans="1:4">
+      <c r="B294" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F294" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6">
       <c r="A295" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="296" spans="1:4">
+    <row r="296" spans="1:6">
       <c r="A296" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="297" spans="1:4">
+    <row r="297" spans="1:6">
       <c r="A297" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="298" spans="1:4">
+      <c r="B297" s="1" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6">
       <c r="A298" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="299" spans="1:4">
+    <row r="299" spans="1:6">
       <c r="A299" t="s">
         <v>302</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D299" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="300" spans="1:4">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6">
       <c r="A300" t="s">
         <v>303</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D300" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6">
       <c r="A301" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="302" spans="1:4">
+    <row r="302" spans="1:6">
       <c r="A302" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="303" spans="1:4">
+    <row r="303" spans="1:6">
       <c r="A303" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="304" spans="1:4">
+    <row r="304" spans="1:6">
       <c r="A304" t="s">
         <v>307</v>
       </c>
@@ -6390,10 +6648,10 @@
         <v>308</v>
       </c>
       <c r="B305" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C305" t="s">
         <v>1068</v>
-      </c>
-      <c r="C305" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -6401,10 +6659,10 @@
         <v>309</v>
       </c>
       <c r="B306" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D306" t="s">
         <v>1070</v>
-      </c>
-      <c r="D306" t="s">
-        <v>1071</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6427,10 +6685,10 @@
         <v>313</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D310" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -6438,7 +6696,7 @@
         <v>314</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -6446,7 +6704,7 @@
         <v>315</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -6464,7 +6722,7 @@
         <v>318</v>
       </c>
       <c r="D315" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6482,7 +6740,7 @@
         <v>321</v>
       </c>
       <c r="B318" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -6490,7 +6748,7 @@
         <v>322</v>
       </c>
       <c r="B319" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -6498,7 +6756,7 @@
         <v>323</v>
       </c>
       <c r="C320" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -6516,7 +6774,7 @@
         <v>326</v>
       </c>
       <c r="D323" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="324" spans="1:6">
@@ -6529,13 +6787,13 @@
         <v>328</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C325" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F325" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="326" spans="1:6">
@@ -6543,13 +6801,13 @@
         <v>329</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C326" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F326" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="327" spans="1:6">
@@ -6557,10 +6815,10 @@
         <v>330</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C327" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="328" spans="1:6">
@@ -6568,10 +6826,10 @@
         <v>331</v>
       </c>
       <c r="B328" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="C328" t="s">
         <v>923</v>
-      </c>
-      <c r="C328" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="329" spans="1:6">
@@ -6579,10 +6837,10 @@
         <v>332</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C329" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="330" spans="1:6">
@@ -6590,10 +6848,10 @@
         <v>333</v>
       </c>
       <c r="B330" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="C330" t="s">
         <v>927</v>
-      </c>
-      <c r="C330" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="331" spans="1:6">
@@ -6601,10 +6859,10 @@
         <v>334</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C331" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="332" spans="1:6">
@@ -6612,10 +6870,10 @@
         <v>335</v>
       </c>
       <c r="B332" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="C332" t="s">
         <v>931</v>
-      </c>
-      <c r="C332" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="333" spans="1:6">
@@ -6638,7 +6896,7 @@
         <v>339</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="337" spans="1:6">
@@ -6646,10 +6904,10 @@
         <v>340</v>
       </c>
       <c r="D337" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F337" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="338" spans="1:6">
@@ -6657,7 +6915,7 @@
         <v>341</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="339" spans="1:6">
@@ -6665,7 +6923,7 @@
         <v>342</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="340" spans="1:6">
@@ -6688,7 +6946,7 @@
         <v>346</v>
       </c>
       <c r="B343" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -6696,7 +6954,7 @@
         <v>347</v>
       </c>
       <c r="F344" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -6704,7 +6962,7 @@
         <v>348</v>
       </c>
       <c r="F345" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="346" spans="1:6">
@@ -6712,7 +6970,7 @@
         <v>349</v>
       </c>
       <c r="F346" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="347" spans="1:6">
@@ -6720,7 +6978,7 @@
         <v>350</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="348" spans="1:6">
@@ -6743,7 +7001,7 @@
         <v>354</v>
       </c>
       <c r="D351" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="352" spans="1:6">
@@ -6751,7 +7009,7 @@
         <v>355</v>
       </c>
       <c r="E352" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="353" spans="1:6">
@@ -6759,7 +7017,7 @@
         <v>356</v>
       </c>
       <c r="C353" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="354" spans="1:6">
@@ -6772,10 +7030,10 @@
         <v>358</v>
       </c>
       <c r="C355" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="F355" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -6783,7 +7041,7 @@
         <v>359</v>
       </c>
       <c r="E356" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -6791,7 +7049,7 @@
         <v>360</v>
       </c>
       <c r="E357" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -6804,7 +7062,7 @@
         <v>362</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="360" spans="1:6">
@@ -6812,7 +7070,7 @@
         <v>363</v>
       </c>
       <c r="D360" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="361" spans="1:6">
@@ -6820,10 +7078,10 @@
         <v>364</v>
       </c>
       <c r="D361" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F361" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="362" spans="1:6">
@@ -6841,10 +7099,10 @@
         <v>369</v>
       </c>
       <c r="C364" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="F364" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="365" spans="1:6">
@@ -6852,7 +7110,7 @@
         <v>367</v>
       </c>
       <c r="C365" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="366" spans="1:6">
@@ -6860,7 +7118,7 @@
         <v>370</v>
       </c>
       <c r="C366" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="367" spans="1:6">
@@ -6868,13 +7126,13 @@
         <v>368</v>
       </c>
       <c r="B367" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C367" t="s">
         <v>970</v>
       </c>
-      <c r="C367" t="s">
-        <v>971</v>
-      </c>
       <c r="F367" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="368" spans="1:6">
@@ -6882,90 +7140,120 @@
         <v>371</v>
       </c>
     </row>
-    <row r="369" spans="1:3">
+    <row r="369" spans="1:6">
       <c r="A369" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:6">
       <c r="A370" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="371" spans="1:3">
+      <c r="D370" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6">
       <c r="A371" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="372" spans="1:3">
+    <row r="372" spans="1:6">
       <c r="A372" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="373" spans="1:3">
+      <c r="B372" s="1" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6">
       <c r="A373" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="374" spans="1:3">
+      <c r="B373" s="1" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6">
       <c r="A374" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="375" spans="1:3">
+      <c r="D374" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F374" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6">
       <c r="A375" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="376" spans="1:3">
+      <c r="B375" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D375" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6">
       <c r="A376" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:6">
       <c r="A377" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:6">
       <c r="A378" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="379" spans="1:3">
+      <c r="F378" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6">
       <c r="A379" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="380" spans="1:3">
+      <c r="B379" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6">
       <c r="A380" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="381" spans="1:3">
+      <c r="D380" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6">
       <c r="A381" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:6">
       <c r="A382" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="383" spans="1:3">
+    <row r="383" spans="1:6">
       <c r="A383" t="s">
         <v>386</v>
       </c>
       <c r="C383" s="1" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="384" spans="1:3">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6">
       <c r="A384" t="s">
         <v>387</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -6973,7 +7261,7 @@
         <v>388</v>
       </c>
       <c r="C385" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -6981,7 +7269,7 @@
         <v>389</v>
       </c>
       <c r="C386" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="387" spans="1:3">
@@ -6989,7 +7277,7 @@
         <v>390</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -6997,7 +7285,7 @@
         <v>391</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="389" spans="1:3">
@@ -7140,7 +7428,7 @@
         <v>419</v>
       </c>
       <c r="C416" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="417" spans="1:5">
@@ -7148,7 +7436,7 @@
         <v>420</v>
       </c>
       <c r="C417" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="418" spans="1:5">
@@ -7156,10 +7444,10 @@
         <v>421</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C418" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="419" spans="1:5">
@@ -7167,10 +7455,10 @@
         <v>422</v>
       </c>
       <c r="B419" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C419" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="420" spans="1:5">
@@ -7178,7 +7466,7 @@
         <v>423</v>
       </c>
       <c r="C420" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="421" spans="1:5">
@@ -7201,7 +7489,7 @@
         <v>427</v>
       </c>
       <c r="C424" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="425" spans="1:5">
@@ -7209,7 +7497,7 @@
         <v>428</v>
       </c>
       <c r="C425" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="426" spans="1:5">
@@ -7217,7 +7505,7 @@
         <v>429</v>
       </c>
       <c r="C426" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="427" spans="1:5">
@@ -7225,7 +7513,7 @@
         <v>430</v>
       </c>
       <c r="E427" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="428" spans="1:5">
@@ -7233,7 +7521,7 @@
         <v>431</v>
       </c>
       <c r="E428" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="429" spans="1:5">
@@ -7241,7 +7529,7 @@
         <v>432</v>
       </c>
       <c r="E429" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="430" spans="1:5">
@@ -7249,7 +7537,7 @@
         <v>433</v>
       </c>
       <c r="E430" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="431" spans="1:5">
@@ -7257,7 +7545,7 @@
         <v>434</v>
       </c>
       <c r="E431" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="432" spans="1:5">
@@ -7265,7 +7553,7 @@
         <v>435</v>
       </c>
       <c r="E432" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="433" spans="1:5">
@@ -7273,7 +7561,7 @@
         <v>436</v>
       </c>
       <c r="E433" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="434" spans="1:5">
@@ -7281,7 +7569,7 @@
         <v>437</v>
       </c>
       <c r="E434" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="435" spans="1:5">
@@ -7289,7 +7577,7 @@
         <v>438</v>
       </c>
       <c r="C435" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="436" spans="1:5">
@@ -7297,7 +7585,7 @@
         <v>439</v>
       </c>
       <c r="E436" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="437" spans="1:5">
@@ -7305,7 +7593,7 @@
         <v>440</v>
       </c>
       <c r="E437" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="438" spans="1:5">
@@ -7313,7 +7601,7 @@
         <v>441</v>
       </c>
       <c r="E438" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="439" spans="1:5">
@@ -7516,10 +7804,10 @@
         <v>482</v>
       </c>
       <c r="B478" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E478" t="s">
         <v>972</v>
-      </c>
-      <c r="E478" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="479" spans="1:5">
@@ -7527,7 +7815,7 @@
         <v>483</v>
       </c>
       <c r="E479" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="480" spans="1:5">
@@ -7535,7 +7823,7 @@
         <v>487</v>
       </c>
       <c r="E480" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="481" spans="1:5">
@@ -7543,7 +7831,7 @@
         <v>484</v>
       </c>
       <c r="E481" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="482" spans="1:5">
@@ -7551,7 +7839,7 @@
         <v>485</v>
       </c>
       <c r="E482" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="483" spans="1:5">
@@ -7559,7 +7847,7 @@
         <v>486</v>
       </c>
       <c r="E483" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="484" spans="1:5">
@@ -7587,7 +7875,7 @@
         <v>492</v>
       </c>
       <c r="D488" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="489" spans="1:5">
@@ -7595,7 +7883,7 @@
         <v>493</v>
       </c>
       <c r="C489" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="490" spans="1:5">
@@ -7603,7 +7891,7 @@
         <v>494</v>
       </c>
       <c r="C490" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="491" spans="1:5">
@@ -7611,7 +7899,7 @@
         <v>495</v>
       </c>
       <c r="C491" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="492" spans="1:5">
@@ -7619,7 +7907,7 @@
         <v>496</v>
       </c>
       <c r="C492" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -7627,7 +7915,7 @@
         <v>497</v>
       </c>
       <c r="C493" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="494" spans="1:5">
@@ -7645,343 +7933,460 @@
         <v>500</v>
       </c>
     </row>
-    <row r="497" spans="1:3">
+    <row r="497" spans="1:6">
       <c r="A497" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="498" spans="1:3">
+    <row r="498" spans="1:6">
       <c r="A498" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="499" spans="1:3">
+    <row r="499" spans="1:6">
       <c r="A499" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="500" spans="1:3">
+    <row r="500" spans="1:6">
       <c r="A500" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="501" spans="1:3">
+    <row r="501" spans="1:6">
       <c r="A501" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="502" spans="1:3">
+    <row r="502" spans="1:6">
       <c r="A502" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="503" spans="1:3">
+    <row r="503" spans="1:6">
       <c r="A503" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="504" spans="1:3">
+    <row r="504" spans="1:6">
       <c r="A504" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="505" spans="1:3">
+    <row r="505" spans="1:6">
       <c r="A505" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="506" spans="1:3">
+    <row r="506" spans="1:6">
       <c r="A506" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="507" spans="1:3">
+    <row r="507" spans="1:6">
       <c r="A507" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="508" spans="1:3">
+    <row r="508" spans="1:6">
       <c r="A508" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="509" spans="1:3">
+    <row r="509" spans="1:6">
       <c r="A509" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="510" spans="1:3">
+    <row r="510" spans="1:6">
       <c r="A510" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="511" spans="1:3">
+    <row r="511" spans="1:6">
       <c r="A511" t="s">
         <v>514</v>
       </c>
       <c r="C511" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="512" spans="1:3">
+        <v>984</v>
+      </c>
+      <c r="F511" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6">
       <c r="A512" t="s">
         <v>515</v>
       </c>
       <c r="C512" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="513" spans="1:3">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6">
       <c r="A513" t="s">
         <v>516</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="514" spans="1:3">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6">
       <c r="A514" t="s">
         <v>517</v>
       </c>
       <c r="C514" s="1" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="515" spans="1:3">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6">
       <c r="A515" t="s">
         <v>518</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="516" spans="1:3">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6">
       <c r="A516" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="517" spans="1:3">
+    <row r="517" spans="1:6">
       <c r="A517" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="518" spans="1:3">
+      <c r="C517" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F517" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6">
       <c r="A518" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="519" spans="1:3">
+      <c r="C518" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F518" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6">
       <c r="A519" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="520" spans="1:3">
+    <row r="520" spans="1:6">
       <c r="A520" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="521" spans="1:3">
+    <row r="521" spans="1:6">
       <c r="A521" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="522" spans="1:3">
+      <c r="E521" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F521" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6">
       <c r="A522" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="523" spans="1:3">
+    <row r="523" spans="1:6">
       <c r="A523" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="524" spans="1:3">
+    <row r="524" spans="1:6">
       <c r="A524" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="525" spans="1:3">
+      <c r="E524" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F524" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6">
       <c r="A525" t="s">
         <v>528</v>
       </c>
       <c r="C525" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="526" spans="1:3">
+        <v>947</v>
+      </c>
+      <c r="F525" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6">
       <c r="A526" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="527" spans="1:3">
+    <row r="527" spans="1:6">
       <c r="A527" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="528" spans="1:3">
+      <c r="D527" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F527" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6">
       <c r="A528" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="529" spans="1:1">
+      <c r="D528" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F528" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6">
       <c r="A529" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="530" spans="1:1">
+    <row r="530" spans="1:6">
       <c r="A530" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="531" spans="1:1">
+    <row r="531" spans="1:6">
       <c r="A531" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="532" spans="1:1">
+      <c r="D531" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6">
       <c r="A532" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="533" spans="1:1">
+    <row r="533" spans="1:6">
       <c r="A533" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="534" spans="1:1">
+    <row r="534" spans="1:6">
       <c r="A534" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="535" spans="1:1">
+      <c r="C534" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F534" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6">
       <c r="A535" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="536" spans="1:1">
+    <row r="536" spans="1:6">
       <c r="A536" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="537" spans="1:1">
+      <c r="D536" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F536" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6">
       <c r="A537" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="538" spans="1:1">
+    <row r="538" spans="1:6">
       <c r="A538" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="539" spans="1:1">
+      <c r="B538" s="1" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6">
       <c r="A539" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="540" spans="1:1">
+      <c r="D539" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F539" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6">
       <c r="A540" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="541" spans="1:1">
+      <c r="D540" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6">
       <c r="A541" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="542" spans="1:1">
+      <c r="D541" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F541" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6">
       <c r="A542" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="543" spans="1:1">
+      <c r="D542" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6">
       <c r="A543" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="544" spans="1:1">
+      <c r="C543" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F543" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6">
       <c r="A544" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="545" spans="1:5">
+      <c r="B544" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6">
       <c r="A545" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="546" spans="1:5">
+    <row r="546" spans="1:6">
       <c r="A546" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="547" spans="1:5">
+      <c r="B546" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6">
       <c r="A547" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="548" spans="1:5">
+      <c r="E547" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F547" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6">
       <c r="A548" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="549" spans="1:5">
+      <c r="D548" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F548" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6">
       <c r="A549" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="550" spans="1:5">
+    <row r="550" spans="1:6">
       <c r="A550" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="551" spans="1:5">
+    <row r="551" spans="1:6">
       <c r="A551" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="552" spans="1:5">
+    <row r="552" spans="1:6">
       <c r="A552" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="553" spans="1:5">
+      <c r="C552" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F552" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6">
       <c r="A553" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="554" spans="1:5">
+      <c r="C553" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F553" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6">
       <c r="A554" t="s">
         <v>557</v>
       </c>
       <c r="E554" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="555" spans="1:5">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6">
       <c r="A555" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="556" spans="1:5">
+    <row r="556" spans="1:6">
       <c r="A556" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="557" spans="1:5">
+    <row r="557" spans="1:6">
       <c r="A557" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="558" spans="1:5">
+    <row r="558" spans="1:6">
       <c r="A558" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="559" spans="1:5">
+    <row r="559" spans="1:6">
       <c r="A559" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="560" spans="1:5">
+    <row r="560" spans="1:6">
       <c r="A560" t="s">
         <v>563</v>
       </c>
@@ -8066,85 +8471,88 @@
         <v>579</v>
       </c>
     </row>
-    <row r="577" spans="1:4">
+    <row r="577" spans="1:6">
       <c r="A577" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="578" spans="1:4">
+    <row r="578" spans="1:6">
       <c r="A578" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="579" spans="1:4">
+    <row r="579" spans="1:6">
       <c r="A579" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="580" spans="1:4">
+    <row r="580" spans="1:6">
       <c r="A580" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="581" spans="1:4">
+    <row r="581" spans="1:6">
       <c r="A581" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="582" spans="1:4">
+    <row r="582" spans="1:6">
       <c r="A582" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="583" spans="1:4">
+    <row r="583" spans="1:6">
       <c r="A583" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="584" spans="1:4">
+    <row r="584" spans="1:6">
       <c r="A584" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="585" spans="1:4">
+    <row r="585" spans="1:6">
       <c r="A585" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="586" spans="1:4">
+    <row r="586" spans="1:6">
       <c r="A586" t="s">
         <v>589</v>
       </c>
       <c r="D586" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F586" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="587" spans="1:4">
+    <row r="587" spans="1:6">
       <c r="A587" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="588" spans="1:4">
+    <row r="588" spans="1:6">
       <c r="A588" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="589" spans="1:4">
+    <row r="589" spans="1:6">
       <c r="A589" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="590" spans="1:4">
+    <row r="590" spans="1:6">
       <c r="A590" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="591" spans="1:4">
+    <row r="591" spans="1:6">
       <c r="A591" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="592" spans="1:4">
+    <row r="592" spans="1:6">
       <c r="A592" t="s">
         <v>595</v>
       </c>
@@ -8153,11 +8561,23 @@
       <c r="A593" t="s">
         <v>596</v>
       </c>
+      <c r="C593" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F593" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="594" spans="1:6">
       <c r="A594" t="s">
         <v>597</v>
       </c>
+      <c r="D594" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F594" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="595" spans="1:6">
       <c r="A595" t="s">
@@ -8168,23 +8588,41 @@
       <c r="A596" t="s">
         <v>599</v>
       </c>
+      <c r="C596" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F596" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="597" spans="1:6">
       <c r="A597" t="s">
         <v>600</v>
       </c>
+      <c r="E597" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F597" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="598" spans="1:6">
       <c r="A598" t="s">
         <v>601</v>
       </c>
+      <c r="E598" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F598" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="599" spans="1:6">
       <c r="A599" t="s">
         <v>602</v>
       </c>
       <c r="C599" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="600" spans="1:6">
@@ -8192,10 +8630,10 @@
         <v>603</v>
       </c>
       <c r="C600" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F600" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="601" spans="1:6">
@@ -8203,7 +8641,7 @@
         <v>604</v>
       </c>
       <c r="C601" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="602" spans="1:6">
@@ -8211,16 +8649,19 @@
         <v>605</v>
       </c>
       <c r="C602" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F602" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="603" spans="1:6">
       <c r="A603" t="s">
         <v>606</v>
       </c>
+      <c r="E603" s="1" t="s">
+        <v>1144</v>
+      </c>
     </row>
     <row r="604" spans="1:6">
       <c r="A604" t="s">
@@ -8231,6 +8672,12 @@
       <c r="A605" t="s">
         <v>608</v>
       </c>
+      <c r="D605" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F605" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="606" spans="1:6">
       <c r="A606" t="s">
@@ -8242,7 +8689,7 @@
         <v>610</v>
       </c>
       <c r="E607" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="608" spans="1:6">
@@ -8250,94 +8697,118 @@
         <v>611</v>
       </c>
     </row>
-    <row r="609" spans="1:5">
+    <row r="609" spans="1:6">
       <c r="A609" t="s">
         <v>612</v>
       </c>
       <c r="E609" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="610" spans="1:5">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6">
       <c r="A610" t="s">
         <v>613</v>
       </c>
       <c r="E610" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="611" spans="1:5">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6">
       <c r="A611" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="612" spans="1:5">
+    <row r="612" spans="1:6">
       <c r="A612" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="613" spans="1:5">
-      <c r="A613" t="s">
+    <row r="613" spans="1:6">
+      <c r="A613" s="1" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="614" spans="1:5">
+      <c r="B613" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E613" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F613" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6">
       <c r="A614" s="1" t="s">
         <v>617</v>
       </c>
       <c r="D614" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="615" spans="1:5">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6">
       <c r="A615" t="s">
         <v>618</v>
       </c>
       <c r="D615" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="616" spans="1:5">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6">
       <c r="A616" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="617" spans="1:5">
+    <row r="617" spans="1:6">
       <c r="A617" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="618" spans="1:5">
+    <row r="618" spans="1:6">
       <c r="A618" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="619" spans="1:5">
+    <row r="619" spans="1:6">
       <c r="A619" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="620" spans="1:5">
+    <row r="620" spans="1:6">
       <c r="A620" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="621" spans="1:5">
+      <c r="B620" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6">
       <c r="A621" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="622" spans="1:5">
+    <row r="622" spans="1:6">
       <c r="A622" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="623" spans="1:5">
+      <c r="D622" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F622" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6">
       <c r="A623" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="624" spans="1:5">
+      <c r="D623" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F623" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6">
       <c r="A624" t="s">
         <v>627</v>
       </c>
@@ -8346,13 +8817,16 @@
       <c r="A625" t="s">
         <v>628</v>
       </c>
+      <c r="B625" s="1" t="s">
+        <v>1151</v>
+      </c>
     </row>
     <row r="626" spans="1:6">
       <c r="A626" t="s">
         <v>629</v>
       </c>
       <c r="D626" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="627" spans="1:6">
@@ -8360,7 +8834,10 @@
         <v>630</v>
       </c>
       <c r="C627" t="s">
-        <v>955</v>
+        <v>954</v>
+      </c>
+      <c r="F627" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="628" spans="1:6">
@@ -8382,13 +8859,16 @@
       <c r="A631" t="s">
         <v>634</v>
       </c>
+      <c r="B631" s="1" t="s">
+        <v>1152</v>
+      </c>
     </row>
     <row r="632" spans="1:6">
       <c r="A632" t="s">
         <v>635</v>
       </c>
       <c r="F632" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="633" spans="1:6">
@@ -8396,7 +8876,7 @@
         <v>636</v>
       </c>
       <c r="F633" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="634" spans="1:6">
@@ -8404,7 +8884,7 @@
         <v>637</v>
       </c>
       <c r="F634" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="635" spans="1:6">
@@ -8412,7 +8892,7 @@
         <v>638</v>
       </c>
       <c r="F635" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="636" spans="1:6">
@@ -8420,7 +8900,7 @@
         <v>639</v>
       </c>
       <c r="F636" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="637" spans="1:6">
@@ -8428,7 +8908,7 @@
         <v>640</v>
       </c>
       <c r="F637" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="638" spans="1:6">
@@ -8436,7 +8916,7 @@
         <v>641</v>
       </c>
       <c r="F638" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="639" spans="1:6">
@@ -8444,7 +8924,7 @@
         <v>642</v>
       </c>
       <c r="F639" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="640" spans="1:6">
@@ -8452,7 +8932,7 @@
         <v>643</v>
       </c>
       <c r="F640" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="641" spans="1:6">
@@ -8460,7 +8940,7 @@
         <v>644</v>
       </c>
       <c r="F641" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="642" spans="1:6">
@@ -8468,37 +8948,64 @@
         <v>645</v>
       </c>
       <c r="F642" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="643" spans="1:6">
       <c r="A643" t="s">
         <v>646</v>
       </c>
+      <c r="B643" s="1" t="s">
+        <v>1153</v>
+      </c>
     </row>
     <row r="644" spans="1:6">
       <c r="A644" t="s">
         <v>647</v>
       </c>
+      <c r="D644" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F644" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="645" spans="1:6">
       <c r="A645" t="s">
         <v>648</v>
       </c>
+      <c r="D645" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F645" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="646" spans="1:6">
       <c r="A646" t="s">
         <v>649</v>
       </c>
+      <c r="B646" s="1" t="s">
+        <v>1156</v>
+      </c>
     </row>
     <row r="647" spans="1:6">
-      <c r="A647" t="s">
+      <c r="A647" s="1" t="s">
         <v>650</v>
       </c>
+      <c r="C647" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F647" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="648" spans="1:6">
-      <c r="A648" t="s">
+      <c r="A648" s="1" t="s">
         <v>651</v>
+      </c>
+      <c r="B648" s="1" t="s">
+        <v>1158</v>
       </c>
     </row>
     <row r="649" spans="1:6">
@@ -8506,10 +9013,10 @@
         <v>652</v>
       </c>
       <c r="E649" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="F649" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="650" spans="1:6">
@@ -8517,10 +9024,10 @@
         <v>653</v>
       </c>
       <c r="E650" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F650" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="651" spans="1:6">
@@ -8528,10 +9035,10 @@
         <v>654</v>
       </c>
       <c r="E651" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F651" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="652" spans="1:6">
@@ -8539,10 +9046,10 @@
         <v>655</v>
       </c>
       <c r="E652" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F652" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="653" spans="1:6">
@@ -8550,10 +9057,10 @@
         <v>656</v>
       </c>
       <c r="E653" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F653" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="654" spans="1:6">
@@ -8561,10 +9068,10 @@
         <v>657</v>
       </c>
       <c r="E654" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F654" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="655" spans="1:6">
@@ -8572,7 +9079,7 @@
         <v>658</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="656" spans="1:6">
@@ -8580,7 +9087,7 @@
         <v>659</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="657" spans="1:6">
@@ -8588,7 +9095,7 @@
         <v>660</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="658" spans="1:6">
@@ -8596,7 +9103,7 @@
         <v>661</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="659" spans="1:6">
@@ -8604,7 +9111,7 @@
         <v>662</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="660" spans="1:6">
@@ -8612,28 +9119,46 @@
         <v>663</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
+      </c>
+      <c r="F660" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="661" spans="1:6">
       <c r="A661" t="s">
         <v>664</v>
       </c>
+      <c r="D661" t="s">
+        <v>1159</v>
+      </c>
     </row>
     <row r="662" spans="1:6">
       <c r="A662" t="s">
         <v>665</v>
       </c>
+      <c r="D662" t="s">
+        <v>1160</v>
+      </c>
     </row>
     <row r="663" spans="1:6">
       <c r="A663" t="s">
         <v>666</v>
       </c>
+      <c r="E663" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F663" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="664" spans="1:6">
       <c r="A664" t="s">
         <v>667</v>
       </c>
+      <c r="B664" s="1" t="s">
+        <v>1162</v>
+      </c>
     </row>
     <row r="665" spans="1:6">
       <c r="A665" t="s">
@@ -8644,6 +9169,12 @@
       <c r="A666" t="s">
         <v>669</v>
       </c>
+      <c r="B666" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E666" t="s">
+        <v>1164</v>
+      </c>
     </row>
     <row r="667" spans="1:6">
       <c r="A667" t="s">
@@ -8655,10 +9186,10 @@
         <v>671</v>
       </c>
       <c r="C668" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F668" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="669" spans="1:6">
@@ -8670,93 +9201,117 @@
       <c r="A670" t="s">
         <v>673</v>
       </c>
+      <c r="C670" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F670" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="671" spans="1:6">
       <c r="A671" t="s">
         <v>674</v>
       </c>
+      <c r="C671" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F671" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="672" spans="1:6">
       <c r="A672" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="673" spans="1:1">
+      <c r="B672" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="673" spans="1:6">
       <c r="A673" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="674" spans="1:1">
+      <c r="B673" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="674" spans="1:6">
       <c r="A674" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="675" spans="1:1">
+      <c r="D674" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F674" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="675" spans="1:6">
       <c r="A675" s="1" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="676" spans="1:1">
+    <row r="676" spans="1:6">
       <c r="A676" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="677" spans="1:1">
+    <row r="677" spans="1:6">
       <c r="A677" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="678" spans="1:1">
+    <row r="678" spans="1:6">
       <c r="A678" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="679" spans="1:1">
+    <row r="679" spans="1:6">
       <c r="A679" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="680" spans="1:1">
+    <row r="680" spans="1:6">
       <c r="A680" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="681" spans="1:1">
+    <row r="681" spans="1:6">
       <c r="A681" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="682" spans="1:1">
+    <row r="682" spans="1:6">
       <c r="A682" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="683" spans="1:1">
+    <row r="683" spans="1:6">
       <c r="A683" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="684" spans="1:1">
+    <row r="684" spans="1:6">
       <c r="A684" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="685" spans="1:1">
+    <row r="685" spans="1:6">
       <c r="A685" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="686" spans="1:1">
+    <row r="686" spans="1:6">
       <c r="A686" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="687" spans="1:1">
+    <row r="687" spans="1:6">
       <c r="A687" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="688" spans="1:1">
+    <row r="688" spans="1:6">
       <c r="A688" t="s">
         <v>691</v>
       </c>
@@ -8896,20 +9451,32 @@
         <v>718</v>
       </c>
       <c r="D715" t="s">
-        <v>1117</v>
+        <v>1116</v>
+      </c>
+      <c r="F715" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="716" spans="1:6">
       <c r="A716" t="s">
         <v>719</v>
       </c>
+      <c r="C716" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D716" t="s">
+        <v>1170</v>
+      </c>
     </row>
     <row r="717" spans="1:6">
       <c r="A717" t="s">
         <v>720</v>
       </c>
       <c r="C717" t="s">
-        <v>1116</v>
+        <v>1115</v>
+      </c>
+      <c r="F717" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="718" spans="1:6">
@@ -8917,10 +9484,10 @@
         <v>721</v>
       </c>
       <c r="D718" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F718" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="719" spans="1:6">
@@ -8928,7 +9495,7 @@
         <v>722</v>
       </c>
       <c r="F719" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="720" spans="1:6">
@@ -8936,7 +9503,7 @@
         <v>723</v>
       </c>
       <c r="F720" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="721" spans="1:6">
@@ -8944,7 +9511,7 @@
         <v>724</v>
       </c>
       <c r="F721" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="722" spans="1:6">
@@ -8952,7 +9519,7 @@
         <v>725</v>
       </c>
       <c r="F722" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="723" spans="1:6">
@@ -8960,7 +9527,7 @@
         <v>726</v>
       </c>
       <c r="F723" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="724" spans="1:6">
@@ -8968,7 +9535,7 @@
         <v>727</v>
       </c>
       <c r="F724" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="725" spans="1:6">
@@ -8976,7 +9543,7 @@
         <v>728</v>
       </c>
       <c r="F725" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="726" spans="1:6">
@@ -8984,7 +9551,7 @@
         <v>729</v>
       </c>
       <c r="F726" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="727" spans="1:6">
@@ -8992,7 +9559,7 @@
         <v>730</v>
       </c>
       <c r="F727" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="728" spans="1:6">
@@ -9000,7 +9567,7 @@
         <v>731</v>
       </c>
       <c r="F728" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="729" spans="1:6">
@@ -9013,10 +9580,10 @@
         <v>253</v>
       </c>
       <c r="C730" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F730" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="731" spans="1:6">
@@ -9024,10 +9591,10 @@
         <v>252</v>
       </c>
       <c r="C731" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F731" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="732" spans="1:6">
@@ -9035,7 +9602,10 @@
         <v>254</v>
       </c>
       <c r="D732" t="s">
-        <v>1115</v>
+        <v>1114</v>
+      </c>
+      <c r="F732" t="s">
+        <v>1172</v>
       </c>
     </row>
     <row r="733" spans="1:6">
@@ -9043,7 +9613,7 @@
         <v>255</v>
       </c>
       <c r="D733" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="734" spans="1:6">
@@ -9051,7 +9621,7 @@
         <v>256</v>
       </c>
       <c r="D734" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="735" spans="1:6">
@@ -9059,7 +9629,7 @@
         <v>733</v>
       </c>
       <c r="F735" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="736" spans="1:6">
@@ -9067,7 +9637,7 @@
         <v>734</v>
       </c>
       <c r="C736" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="737" spans="1:6">
@@ -9075,7 +9645,7 @@
         <v>735</v>
       </c>
       <c r="C737" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="738" spans="1:6">
@@ -9083,7 +9653,7 @@
         <v>736</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="739" spans="1:6">
@@ -9091,7 +9661,7 @@
         <v>737</v>
       </c>
       <c r="C739" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="740" spans="1:6">
@@ -9099,7 +9669,7 @@
         <v>738</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="741" spans="1:6">
@@ -9107,7 +9677,7 @@
         <v>739</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="742" spans="1:6">
@@ -9115,10 +9685,10 @@
         <v>740</v>
       </c>
       <c r="C742" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F742" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="743" spans="1:6">
@@ -9126,10 +9696,10 @@
         <v>741</v>
       </c>
       <c r="D743" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F743" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="744" spans="1:6">
@@ -9137,7 +9707,7 @@
         <v>742</v>
       </c>
       <c r="D744" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="745" spans="1:6">
@@ -9145,51 +9715,69 @@
         <v>743</v>
       </c>
       <c r="E745" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="746" spans="1:6">
       <c r="A746" t="s">
         <v>744</v>
       </c>
+      <c r="B746" t="s">
+        <v>1173</v>
+      </c>
     </row>
     <row r="747" spans="1:6">
       <c r="A747" t="s">
         <v>745</v>
       </c>
       <c r="D747" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="748" spans="1:6">
       <c r="A748" t="s">
         <v>746</v>
       </c>
+      <c r="B748" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C748" t="s">
+        <v>1175</v>
+      </c>
     </row>
     <row r="749" spans="1:6">
       <c r="A749" t="s">
         <v>747</v>
       </c>
+      <c r="C749" t="s">
+        <v>1176</v>
+      </c>
     </row>
     <row r="750" spans="1:6">
       <c r="A750" t="s">
         <v>748</v>
       </c>
+      <c r="D750" t="s">
+        <v>1177</v>
+      </c>
     </row>
     <row r="751" spans="1:6">
       <c r="A751" t="s">
         <v>749</v>
       </c>
+      <c r="B751" s="1" t="s">
+        <v>1178</v>
+      </c>
     </row>
     <row r="752" spans="1:6">
       <c r="A752" t="s">
         <v>750</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="F752" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="753" spans="1:6">
@@ -9197,10 +9785,10 @@
         <v>751</v>
       </c>
       <c r="C753" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F753" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="754" spans="1:6">
@@ -9208,10 +9796,10 @@
         <v>752</v>
       </c>
       <c r="C754" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F754" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="755" spans="1:6">
@@ -9223,22 +9811,22 @@
       <c r="A756" t="s">
         <v>754</v>
       </c>
+      <c r="B756" s="1" t="s">
+        <v>1108</v>
+      </c>
     </row>
     <row r="757" spans="1:6">
       <c r="A757" t="s">
         <v>755</v>
       </c>
-      <c r="B757" s="1" t="s">
-        <v>1109</v>
+      <c r="D757" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="758" spans="1:6">
       <c r="A758" t="s">
         <v>756</v>
       </c>
-      <c r="D758" t="s">
-        <v>1108</v>
-      </c>
     </row>
     <row r="759" spans="1:6">
       <c r="A759" t="s">
@@ -9249,44 +9837,65 @@
       <c r="A760" t="s">
         <v>758</v>
       </c>
+      <c r="F760" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="761" spans="1:6">
       <c r="A761" t="s">
         <v>759</v>
       </c>
+      <c r="F761" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="762" spans="1:6">
       <c r="A762" t="s">
         <v>760</v>
       </c>
+      <c r="C762" t="s">
+        <v>1179</v>
+      </c>
     </row>
     <row r="763" spans="1:6">
       <c r="A763" t="s">
         <v>761</v>
       </c>
+      <c r="B763" s="1" t="s">
+        <v>1180</v>
+      </c>
     </row>
     <row r="764" spans="1:6">
       <c r="A764" t="s">
         <v>762</v>
       </c>
+      <c r="D764" t="s">
+        <v>1011</v>
+      </c>
     </row>
     <row r="765" spans="1:6">
       <c r="A765" t="s">
         <v>763</v>
       </c>
-      <c r="D765" t="s">
-        <v>1012</v>
+      <c r="B765" s="1" t="s">
+        <v>1181</v>
       </c>
     </row>
     <row r="766" spans="1:6">
       <c r="A766" t="s">
         <v>764</v>
       </c>
+      <c r="C766" t="s">
+        <v>1182</v>
+      </c>
     </row>
     <row r="767" spans="1:6">
       <c r="A767" t="s">
         <v>765</v>
       </c>
+      <c r="C767" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="768" spans="1:6">
       <c r="A768" t="s">
@@ -9303,27 +9912,30 @@
       <c r="C769" t="s">
         <v>1007</v>
       </c>
+      <c r="F769" t="s">
+        <v>1008</v>
+      </c>
     </row>
     <row r="770" spans="1:6">
       <c r="A770" t="s">
         <v>768</v>
       </c>
       <c r="C770" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="F770" t="s">
-        <v>1009</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="771" spans="1:6">
       <c r="A771" t="s">
         <v>769</v>
       </c>
-      <c r="C771" t="s">
-        <v>1010</v>
+      <c r="D771" t="s">
+        <v>1099</v>
       </c>
       <c r="F771" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="772" spans="1:6">
@@ -9331,10 +9943,7 @@
         <v>770</v>
       </c>
       <c r="D772" t="s">
-        <v>1100</v>
-      </c>
-      <c r="F772" t="s">
-        <v>1028</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="773" spans="1:6">
@@ -9342,7 +9951,7 @@
         <v>771</v>
       </c>
       <c r="D773" t="s">
-        <v>1107</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="774" spans="1:6">
@@ -9350,16 +9959,13 @@
         <v>772</v>
       </c>
       <c r="D774" t="s">
-        <v>1013</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="775" spans="1:6">
       <c r="A775" t="s">
         <v>773</v>
       </c>
-      <c r="D775" t="s">
-        <v>1106</v>
-      </c>
     </row>
     <row r="776" spans="1:6">
       <c r="A776" t="s">
@@ -9370,14 +9976,14 @@
       <c r="A777" t="s">
         <v>775</v>
       </c>
+      <c r="D777" t="s">
+        <v>1104</v>
+      </c>
     </row>
     <row r="778" spans="1:6">
       <c r="A778" t="s">
         <v>776</v>
       </c>
-      <c r="D778" t="s">
-        <v>1105</v>
-      </c>
     </row>
     <row r="779" spans="1:6">
       <c r="A779" t="s">
@@ -9403,42 +10009,37 @@
       <c r="A783" t="s">
         <v>781</v>
       </c>
+      <c r="D783" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="784" spans="1:6">
       <c r="A784" t="s">
         <v>782</v>
       </c>
-      <c r="D784" t="s">
-        <v>1011</v>
-      </c>
     </row>
     <row r="785" spans="1:6">
       <c r="A785" t="s">
         <v>783</v>
       </c>
+      <c r="F785" t="s">
+        <v>1094</v>
+      </c>
     </row>
     <row r="786" spans="1:6">
       <c r="A786" t="s">
         <v>784</v>
       </c>
       <c r="F786" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="787" spans="1:6">
       <c r="A787" t="s">
-        <v>785</v>
-      </c>
-      <c r="F787" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="788" spans="1:6">
-      <c r="A788" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D787" t="s">
         <v>1103</v>
-      </c>
-      <c r="D788" t="s">
-        <v>1104</v>
       </c>
     </row>
   </sheetData>
@@ -9570,12 +10171,42 @@
     <hyperlink ref="A675" r:id="rId125" xr:uid="{04CF27F5-B4E7-40B2-A365-8B8880E60B95}"/>
     <hyperlink ref="C752" r:id="rId126" xr:uid="{85B3017C-57A5-4315-8634-50A155E99DBA}"/>
     <hyperlink ref="A614" r:id="rId127" xr:uid="{BE4A11B8-840F-4E92-B887-31ACA717F219}"/>
-    <hyperlink ref="B757" r:id="rId128" display="https://doi.org/10.18311/jims/1942/17182" xr:uid="{6896B2FF-215B-424F-8E91-DAF3FB5B8026}"/>
+    <hyperlink ref="B756" r:id="rId128" display="https://doi.org/10.18311/jims/1942/17182" xr:uid="{6896B2FF-215B-424F-8E91-DAF3FB5B8026}"/>
+    <hyperlink ref="B538" r:id="rId129" display="http://www.nist.gov/dads/HTML/hammingdist.html" xr:uid="{D5C4107B-6CFA-4313-8AC7-7976AFBC99CA}"/>
+    <hyperlink ref="B544" r:id="rId130" display="http://www.oberlin.edu/math/faculty/wilmer/OEISconj727374.pdf" xr:uid="{E8F3780B-3BC6-4E9B-9CB9-DBC9B30BC494}"/>
+    <hyperlink ref="B546" r:id="rId131" display="http://www.olemiss.edu/mathed/pow/november.html" xr:uid="{1F9DE618-7D91-4108-AA26-DA148B7FFCE4}"/>
+    <hyperlink ref="E524" r:id="rId132" xr:uid="{6A3B0065-F789-42AB-9C79-4B7063D50E62}"/>
+    <hyperlink ref="D594" r:id="rId133" xr:uid="{118AB257-5C3F-44F3-8234-040FF5EA73F8}"/>
+    <hyperlink ref="E603" r:id="rId134" xr:uid="{746A1CB2-C795-4C43-9EE8-E04BA3F5B96E}"/>
+    <hyperlink ref="B613" r:id="rId135" display="http://www.sci.brooklyn.cuny.edu/~amotz/GC-ALGORITHMS/PRESENTATIONS/" xr:uid="{FD3D951F-B1ED-4CB3-9B99-631BA93FC91F}"/>
+    <hyperlink ref="A613" r:id="rId136" xr:uid="{E52E9CE2-B56D-4F84-9979-43B9E5B6A57A}"/>
+    <hyperlink ref="B620" r:id="rId137" display="http://www.seds.org/nineplanets/nineplanets/nineplanets.html" xr:uid="{9AF7C2C1-37AE-4544-BEDD-0F0F2E737766}"/>
+    <hyperlink ref="B625" r:id="rId138" display="http://www.skidmore.edu/academics/mcs/pme913.htm" xr:uid="{815A1150-6551-41BF-B023-0EF9D06AE5A5}"/>
+    <hyperlink ref="B631" r:id="rId139" display="http://www.squareonetv.org/default.asp?ID=17" xr:uid="{C5D8A807-1675-48EA-9132-A79300429C50}"/>
+    <hyperlink ref="B643" r:id="rId140" display="http://www.swox.com/gmp/repunit.html" xr:uid="{1EC36F43-CC12-43F3-9D7E-11994A3A6239}"/>
+    <hyperlink ref="B646" r:id="rId141" display="http://www.time.com/time/specials/2007/article/0,28804,1815747_1815707_1815674,00.html" xr:uid="{E2C39E7D-5D7A-4368-A87C-12E5ECFC2DFA}"/>
+    <hyperlink ref="A647" r:id="rId142" xr:uid="{1985E327-C93D-479B-A089-A4E0447AC1DF}"/>
+    <hyperlink ref="A648" r:id="rId143" xr:uid="{53C0118A-4EC7-4211-9813-C5E700DA7747}"/>
+    <hyperlink ref="B648" r:id="rId144" display="http://www.tower.com/tower_search/search_1.cfm?keywords=beethoven%205th" xr:uid="{DFBEBBCE-CD78-4AF4-9E79-1F7F1375D0B2}"/>
+    <hyperlink ref="B664" r:id="rId145" display="http://www.uni-graz.at/~fripert/fga/k1euler.html" xr:uid="{78D5A552-232D-4310-9800-B01F4C624A29}"/>
+    <hyperlink ref="B666" r:id="rId146" display="http://www.users.zetnet.co.uk/egrichards/book.htm" xr:uid="{07938A4E-2AE8-43AA-BD6E-DB8DAD840E44}"/>
+    <hyperlink ref="B673" r:id="rId147" display="http://www.westfield.ma.edu/math/faculty/jaiclin/writings/research/pascals_triangle/" xr:uid="{5761F8B8-79FE-4E58-8CA6-DA6379AAB75D}"/>
+    <hyperlink ref="B748" r:id="rId148" display="https://cs.uwaterloo.ca/journals/JIS/OL13/Pan/pan8.html" xr:uid="{6BDB86A1-A564-4273-BC96-18A58D666457}"/>
+    <hyperlink ref="B751" r:id="rId149" display="https://dl.dropbox.com/u/46675017/Graph %28A%28n%29-2n%29%3Asqrt%28n%29.png" xr:uid="{418B68E1-D1C1-483F-8374-D849A04329BF}"/>
+    <hyperlink ref="B763" r:id="rId150" display="https://math.hawaii.edu/~bjoern/Publications/BKY-June-2018.pdf" xr:uid="{51F5554F-56CE-4431-BFBE-E4C0B3D5EA35}"/>
+    <hyperlink ref="B765" r:id="rId151" display="https://mathoverflow.net/questions/331170" xr:uid="{C90062BC-7FAF-4A9A-8688-A3E3BA456BA2}"/>
+    <hyperlink ref="B372" r:id="rId152" display="http://www.icm.tu-bs.de/ag_algebra/software/small/number.html" xr:uid="{E87D7E74-F9AF-4A6C-8181-BB5DD36E10D4}"/>
+    <hyperlink ref="B373" r:id="rId153" display="http://www.icm.tu-bs.de/ag_algebra/software/small/small.html" xr:uid="{0C8025FC-5D72-48CD-9B61-86FAFB634D54}"/>
+    <hyperlink ref="B375" r:id="rId154" display="http://www.ift.uni.wroc.pl/~mwolf/" xr:uid="{C749CAB6-B5D1-406D-B6BD-2DCB16A703DE}"/>
+    <hyperlink ref="B297" r:id="rId155" display="http://www.coin-gallery.com/cguscoinage.htm" xr:uid="{B387FF4D-3BB1-4FF7-BAF5-D94D8C6C5C42}"/>
+    <hyperlink ref="B294" r:id="rId156" display="http://www.cmb.usc.edu/people/msw/Waterman.html" xr:uid="{49F8E4A5-D560-4F65-A06A-E94ABB0279F6}"/>
+    <hyperlink ref="B288" r:id="rId157" display="http://www.chf.nu/CHF_DIATOMIC_ALGORITHM_BENCHMARK.pdf" xr:uid="{69A12494-E8A2-4980-9AE6-814ED6BB1958}"/>
+    <hyperlink ref="B287" r:id="rId158" location="62" display="http://www.chalcedon.demon.co.uk/publish.html - 62" xr:uid="{69CF8CDB-5FFD-4C2F-8729-40126929F5CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId129"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId159"/>
   <tableParts count="1">
-    <tablePart r:id="rId130"/>
+    <tablePart r:id="rId160"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>